<commit_message>
60 more datasets generated and added to excel sheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,41 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saswat\Desktop\KnockMLDatasetGeneration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DC1259-5EFB-489F-9077-14BB6C74DCFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Amplitude</t>
-  </si>
-  <si>
-    <t>Phase</t>
-  </si>
-  <si>
-    <t>Tempo</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +58,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -118,7 +112,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -150,9 +144,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,6 +196,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -359,22 +389,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>12.20793397875834</v>
+        <v>12.207933978758341</v>
       </c>
       <c r="B1">
-        <v>31.15882422761533</v>
+        <v>31.158824221723918</v>
       </c>
       <c r="C1">
-        <v>43.48169544805705</v>
+        <v>43.486968097800784</v>
       </c>
       <c r="D1">
         <v>161.4990234375</v>
@@ -383,49 +415,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9.027216581157859</v>
+        <v>9.0272165811578589</v>
       </c>
       <c r="B2">
-        <v>27.38100625733735</v>
+        <v>27.381006255621902</v>
       </c>
       <c r="C2">
-        <v>42.5116625914389</v>
+        <v>42.523310884066412</v>
       </c>
       <c r="D2">
-        <v>112.3471467391304</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11.08065093346771</v>
+        <v>11.080650933467711</v>
       </c>
       <c r="B3">
-        <v>29.76354408787492</v>
+        <v>29.76354408711169</v>
       </c>
       <c r="C3">
-        <v>40.98284590667019</v>
+        <v>40.963686312294342</v>
       </c>
       <c r="D3">
-        <v>198.7680288461538</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>16.68356557877621</v>
+        <v>16.68356557880529</v>
       </c>
       <c r="B4">
-        <v>41.62095830330234</v>
+        <v>41.620958322188947</v>
       </c>
       <c r="C4">
-        <v>48.97553846146094</v>
+        <v>48.985580429468172</v>
       </c>
       <c r="D4">
         <v>161.4990234375</v>
@@ -434,15 +466,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16.7137039099755</v>
       </c>
       <c r="B5">
-        <v>36.85226522818317</v>
+        <v>36.852265219518692</v>
       </c>
       <c r="C5">
-        <v>50.92307215797731</v>
+        <v>50.915033584508578</v>
       </c>
       <c r="D5">
         <v>151.9990808823529</v>
@@ -451,15 +483,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10.30867307217921</v>
+        <v>10.308673072178751</v>
       </c>
       <c r="B6">
-        <v>28.85081096364281</v>
+        <v>28.850810959942969</v>
       </c>
       <c r="C6">
-        <v>49.89040482513266</v>
+        <v>49.885919312899837</v>
       </c>
       <c r="D6">
         <v>103.359375</v>
@@ -468,15 +500,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8.610503085037688</v>
+        <v>8.6105030850522262</v>
       </c>
       <c r="B7">
-        <v>25.29926216776829</v>
+        <v>25.299262163450589</v>
       </c>
       <c r="C7">
-        <v>43.97272358657066</v>
+        <v>43.970209075691322</v>
       </c>
       <c r="D7">
         <v>103.359375</v>
@@ -485,15 +517,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10.47633707116122</v>
       </c>
       <c r="B8">
-        <v>27.09750285545265</v>
+        <v>27.097502847925739</v>
       </c>
       <c r="C8">
-        <v>39.37236978035877</v>
+        <v>39.370375152842463</v>
       </c>
       <c r="D8">
         <v>129.19921875</v>
@@ -502,32 +534,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11.38424189675722</v>
+        <v>11.38424189674268</v>
       </c>
       <c r="B9">
-        <v>26.72121182785648</v>
+        <v>26.72121182224674</v>
       </c>
       <c r="C9">
-        <v>40.90835034344946</v>
+        <v>40.91013873046623</v>
       </c>
       <c r="D9">
-        <v>117.4538352272727</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11.48621191781259</v>
+        <v>11.486211917823489</v>
       </c>
       <c r="B10">
-        <v>34.62951405293749</v>
+        <v>34.62951404590715</v>
       </c>
       <c r="C10">
-        <v>48.06314097562951</v>
+        <v>48.069561029250607</v>
       </c>
       <c r="D10">
         <v>143.5546875</v>
@@ -536,15 +568,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8.008719178920234</v>
+        <v>8.0087191789202343</v>
       </c>
       <c r="B11">
-        <v>22.15405397569183</v>
+        <v>22.154053972843801</v>
       </c>
       <c r="C11">
-        <v>32.47210926723487</v>
+        <v>32.4665903079419</v>
       </c>
       <c r="D11">
         <v>151.9990808823529</v>
@@ -553,15 +585,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5.319798594193406</v>
+        <v>5.3197985941934061</v>
       </c>
       <c r="B12">
-        <v>16.54442632209611</v>
+        <v>16.544426321543678</v>
       </c>
       <c r="C12">
-        <v>28.39685565121053</v>
+        <v>28.40577999519401</v>
       </c>
       <c r="D12">
         <v>143.5546875</v>
@@ -570,15 +602,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6.415760074822061</v>
+        <v>6.4157600748220611</v>
       </c>
       <c r="B13">
-        <v>20.29118659913855</v>
+        <v>20.291186597306801</v>
       </c>
       <c r="C13">
-        <v>32.45631936191587</v>
+        <v>32.453595921390139</v>
       </c>
       <c r="D13">
         <v>151.9990808823529</v>
@@ -587,15 +619,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4.562605658782881</v>
+        <v>4.5626056587824264</v>
       </c>
       <c r="B14">
-        <v>17.33822821953827</v>
+        <v>17.338228218724161</v>
       </c>
       <c r="C14">
-        <v>28.95084281726564</v>
+        <v>28.927344406814139</v>
       </c>
       <c r="D14">
         <v>103.359375</v>
@@ -604,15 +636,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>8.236140772218327</v>
+        <v>8.2361407722185547</v>
       </c>
       <c r="B15">
-        <v>25.43869137404376</v>
+        <v>25.4386913714924</v>
       </c>
       <c r="C15">
-        <v>38.96081270500398</v>
+        <v>38.94734749929831</v>
       </c>
       <c r="D15">
         <v>107.666015625</v>
@@ -621,15 +653,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8.021787065581513</v>
+        <v>8.0217870655815702</v>
       </c>
       <c r="B16">
-        <v>22.94728056146079</v>
+        <v>22.947280559311029</v>
       </c>
       <c r="C16">
-        <v>38.45198139794946</v>
+        <v>38.458921919387009</v>
       </c>
       <c r="D16">
         <v>151.9990808823529</v>
@@ -638,15 +670,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>8.045097591888711</v>
+        <v>8.0450975918850762</v>
       </c>
       <c r="B17">
-        <v>24.0169972034564</v>
+        <v>24.016997200347149</v>
       </c>
       <c r="C17">
-        <v>38.54181242613359</v>
+        <v>38.545769830713411</v>
       </c>
       <c r="D17">
         <v>215.33203125</v>
@@ -655,15 +687,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>7.646895599282701</v>
+        <v>7.6468955992826864</v>
       </c>
       <c r="B18">
-        <v>22.34456282069589</v>
+        <v>22.34456281936933</v>
       </c>
       <c r="C18">
-        <v>34.45965470546538</v>
+        <v>34.462563191647519</v>
       </c>
       <c r="D18">
         <v>123.046875</v>
@@ -672,15 +704,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7.901829908435769</v>
+        <v>7.9018299084357686</v>
       </c>
       <c r="B19">
-        <v>26.28014279572675</v>
+        <v>26.280142793695109</v>
       </c>
       <c r="C19">
-        <v>37.0031209812201</v>
+        <v>37.007836202058712</v>
       </c>
       <c r="D19">
         <v>107.666015625</v>
@@ -689,15 +721,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5.802652517905123</v>
+        <v>5.8026525179051234</v>
       </c>
       <c r="B20">
-        <v>25.75464201748123</v>
+        <v>25.75464201939657</v>
       </c>
       <c r="C20">
-        <v>36.94502044900754</v>
+        <v>36.948889560210567</v>
       </c>
       <c r="D20">
         <v>143.5546875</v>
@@ -706,15 +738,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9.386360785119233</v>
+        <v>9.3863607851169633</v>
       </c>
       <c r="B21">
-        <v>30.0594356803487</v>
+        <v>30.05943567999979</v>
       </c>
       <c r="C21">
-        <v>42.49475188175502</v>
+        <v>42.485767903670506</v>
       </c>
       <c r="D21">
         <v>143.5546875</v>
@@ -723,32 +755,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7.032261608127743</v>
+        <v>7.0322616081352392</v>
       </c>
       <c r="B22">
-        <v>19.82470008483671</v>
+        <v>19.824700079752141</v>
       </c>
       <c r="C22">
-        <v>36.10425737640895</v>
+        <v>36.116781705269979</v>
       </c>
       <c r="D22">
-        <v>135.999177631579</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5.607066680648122</v>
+        <v>5.6070666806481224</v>
       </c>
       <c r="B23">
-        <v>23.25354732684951</v>
+        <v>23.253547326020861</v>
       </c>
       <c r="C23">
-        <v>34.4541404810105</v>
+        <v>34.467388321699858</v>
       </c>
       <c r="D23">
         <v>172.265625</v>
@@ -757,15 +789,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>6.71230209169426</v>
+        <v>6.7123020916941467</v>
       </c>
       <c r="B24">
-        <v>21.83760330087329</v>
+        <v>21.83760329880894</v>
       </c>
       <c r="C24">
-        <v>32.52543393881171</v>
+        <v>32.519685036464637</v>
       </c>
       <c r="D24">
         <v>143.5546875</v>
@@ -774,15 +806,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>10.43563062198517</v>
+        <v>10.435630621990329</v>
       </c>
       <c r="B25">
-        <v>29.24294621645317</v>
+        <v>29.24294621450829</v>
       </c>
       <c r="C25">
-        <v>38.45537827849247</v>
+        <v>38.449738620713248</v>
       </c>
       <c r="D25">
         <v>143.5546875</v>
@@ -791,15 +823,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>7.988779991359279</v>
+        <v>7.9887799913592792</v>
       </c>
       <c r="B26">
-        <v>22.28739511998446</v>
+        <v>22.287395115157938</v>
       </c>
       <c r="C26">
-        <v>32.9476196856476</v>
+        <v>32.938789923250873</v>
       </c>
       <c r="D26">
         <v>151.9990808823529</v>
@@ -808,15 +840,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>6.092986008292811</v>
+        <v>6.092986008292697</v>
       </c>
       <c r="B27">
-        <v>19.79685912134506</v>
+        <v>19.796859119338858</v>
       </c>
       <c r="C27">
-        <v>33.02193261392865</v>
+        <v>33.01676530885608</v>
       </c>
       <c r="D27">
         <v>143.5546875</v>
@@ -825,15 +857,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>8.261867727164041</v>
+        <v>8.2618677271640983</v>
       </c>
       <c r="B28">
-        <v>24.6737586808643</v>
+        <v>24.67375867885082</v>
       </c>
       <c r="C28">
-        <v>38.51092644179085</v>
+        <v>38.515744386381591</v>
       </c>
       <c r="D28">
         <v>123.046875</v>
@@ -842,15 +874,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>6.473021174833161</v>
+        <v>6.4730211748331614</v>
       </c>
       <c r="B29">
-        <v>27.48818425951809</v>
+        <v>27.48818425779173</v>
       </c>
       <c r="C29">
-        <v>34.46836434932094</v>
+        <v>34.486773025201913</v>
       </c>
       <c r="D29">
         <v>143.5546875</v>
@@ -859,15 +891,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>6.474187113410025</v>
+        <v>6.4741871134093438</v>
       </c>
       <c r="B30">
-        <v>21.57744873457057</v>
+        <v>21.577448733102251</v>
       </c>
       <c r="C30">
-        <v>38.52642701501239</v>
+        <v>38.526859392719459</v>
       </c>
       <c r="D30">
         <v>151.9990808823529</v>
@@ -876,15 +908,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5.953082456829551</v>
+        <v>5.9530824568297778</v>
       </c>
       <c r="B31">
-        <v>20.22091594859547</v>
+        <v>20.220915947519671</v>
       </c>
       <c r="C31">
-        <v>35.46639279430872</v>
+        <v>35.455778845739552</v>
       </c>
       <c r="D31">
         <v>161.4990234375</v>
@@ -893,15 +925,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>6.01825900943042</v>
+        <v>6.0182590094305048</v>
       </c>
       <c r="B32">
-        <v>17.69960660454774</v>
+        <v>17.699606603344741</v>
       </c>
       <c r="C32">
-        <v>32.47291282544538</v>
+        <v>32.464518842438899</v>
       </c>
       <c r="D32">
         <v>143.5546875</v>
@@ -910,15 +942,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9.442022761919183</v>
+        <v>9.4420227619200858</v>
       </c>
       <c r="B33">
-        <v>19.48669792330489</v>
+        <v>19.486697921961969</v>
       </c>
       <c r="C33">
-        <v>34.51381857687165</v>
+        <v>34.505199289614268</v>
       </c>
       <c r="D33">
         <v>143.5546875</v>
@@ -927,15 +959,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3.742724841615818</v>
+        <v>3.7427248416158179</v>
       </c>
       <c r="B34">
-        <v>12.10796329922537</v>
+        <v>12.107963297650761</v>
       </c>
       <c r="C34">
-        <v>33.95771691037032</v>
+        <v>33.964322679850817</v>
       </c>
       <c r="D34">
         <v>143.5546875</v>
@@ -944,15 +976,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>8.631738708572071</v>
+        <v>8.6317387085714046</v>
       </c>
       <c r="B35">
-        <v>36.13234280826562</v>
+        <v>36.132342807291593</v>
       </c>
       <c r="C35">
-        <v>36.96314053383156</v>
+        <v>36.961703901971923</v>
       </c>
       <c r="D35">
         <v>151.9990808823529</v>
@@ -961,32 +993,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9.235046398989921</v>
+        <v>9.2350463989826519</v>
       </c>
       <c r="B36">
-        <v>28.75157577019947</v>
+        <v>28.751575764275319</v>
       </c>
       <c r="C36">
-        <v>37.50123301942699</v>
+        <v>37.495795349310612</v>
       </c>
       <c r="D36">
-        <v>112.3471467391304</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>8.330172942564305</v>
+        <v>8.3301729425647597</v>
       </c>
       <c r="B37">
-        <v>32.13771244986975</v>
+        <v>32.137712447610951</v>
       </c>
       <c r="C37">
-        <v>50.01153877503443</v>
+        <v>50.001756461295628</v>
       </c>
       <c r="D37">
         <v>143.5546875</v>
@@ -995,15 +1027,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>6.915895499198408</v>
+        <v>6.9158954991965906</v>
       </c>
       <c r="B38">
-        <v>30.32702352849321</v>
+        <v>30.32702352611448</v>
       </c>
       <c r="C38">
-        <v>37.92040398234455</v>
+        <v>37.924022565638808</v>
       </c>
       <c r="D38">
         <v>73.828125</v>
@@ -1012,15 +1044,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6.092609462980052</v>
       </c>
       <c r="B39">
-        <v>20.34202310843061</v>
+        <v>20.34202310713675</v>
       </c>
       <c r="C39">
-        <v>34.45534357835425</v>
+        <v>34.443780104971822</v>
       </c>
       <c r="D39">
         <v>123.046875</v>
@@ -1029,15 +1061,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>8.426739708832629</v>
+        <v>8.4267397088328568</v>
       </c>
       <c r="B40">
-        <v>25.23276066332156</v>
+        <v>25.232760662107658</v>
       </c>
       <c r="C40">
-        <v>36.53779385067216</v>
+        <v>36.5214782319091</v>
       </c>
       <c r="D40">
         <v>151.9990808823529</v>
@@ -1046,15 +1078,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5.492538208569048</v>
       </c>
       <c r="B41">
-        <v>21.55605498824728</v>
+        <v>21.556054986619959</v>
       </c>
       <c r="C41">
-        <v>34.95851054110033</v>
+        <v>34.958524604244381</v>
       </c>
       <c r="D41">
         <v>86.1328125</v>
@@ -1063,15 +1095,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>6.382900157246535</v>
+        <v>6.3829001572460813</v>
       </c>
       <c r="B42">
-        <v>20.39462244186319</v>
+        <v>20.3946224416006</v>
       </c>
       <c r="C42">
-        <v>39.89038416570737</v>
+        <v>39.891949610176852</v>
       </c>
       <c r="D42">
         <v>143.5546875</v>
@@ -1080,15 +1112,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>7.213539063889312</v>
+        <v>7.2135390638864729</v>
       </c>
       <c r="B43">
-        <v>21.59045773489964</v>
+        <v>21.590457733649401</v>
       </c>
       <c r="C43">
-        <v>36.46238237811738</v>
+        <v>36.456509333234692</v>
       </c>
       <c r="D43">
         <v>103.359375</v>
@@ -1097,15 +1129,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>9.626021097970268</v>
+        <v>9.6260210979700478</v>
       </c>
       <c r="B44">
-        <v>25.07505080813802</v>
+        <v>25.07505080532497</v>
       </c>
       <c r="C44">
-        <v>36.97014849234773</v>
+        <v>36.955946186222953</v>
       </c>
       <c r="D44">
         <v>143.5546875</v>
@@ -1114,15 +1146,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>6.587153528556621</v>
+        <v>6.5871535285420837</v>
       </c>
       <c r="B45">
-        <v>22.36757545852363</v>
+        <v>22.367575456786369</v>
       </c>
       <c r="C45">
-        <v>34.01303338062255</v>
+        <v>34.020614196311158</v>
       </c>
       <c r="D45">
         <v>161.4990234375</v>
@@ -1131,15 +1163,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>7.811970927391926</v>
+        <v>7.8119709273937428</v>
       </c>
       <c r="B46">
-        <v>32.45305215708529</v>
+        <v>32.453052151808997</v>
       </c>
       <c r="C46">
-        <v>36.0151422610527</v>
+        <v>36.018890659344031</v>
       </c>
       <c r="D46">
         <v>151.9990808823529</v>
@@ -1148,15 +1180,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>7.790261679061751</v>
+        <v>7.7902616791126329</v>
       </c>
       <c r="B47">
-        <v>31.63863718092528</v>
+        <v>31.63863717845387</v>
       </c>
       <c r="C47">
-        <v>37.5335432615475</v>
+        <v>37.522729055934661</v>
       </c>
       <c r="D47">
         <v>161.4990234375</v>
@@ -1165,32 +1197,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6.837257407660543</v>
+        <v>6.8372574076607124</v>
       </c>
       <c r="B48">
-        <v>19.78564299866673</v>
+        <v>19.785642996173522</v>
       </c>
       <c r="C48">
-        <v>38.50220714105378</v>
+        <v>38.4927067156828</v>
       </c>
       <c r="D48">
-        <v>117.4538352272727</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>10.0813179548836</v>
+        <v>10.081317954890871</v>
       </c>
       <c r="B49">
-        <v>36.24837994433292</v>
+        <v>36.248379942108649</v>
       </c>
       <c r="C49">
-        <v>37.47420368784997</v>
+        <v>37.493748489034957</v>
       </c>
       <c r="D49">
         <v>107.666015625</v>
@@ -1199,32 +1231,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>5.709635090319338</v>
+        <v>5.7096350903209281</v>
       </c>
       <c r="B50">
-        <v>19.26767504607847</v>
+        <v>19.26767504450839</v>
       </c>
       <c r="C50">
-        <v>35.41858800414493</v>
+        <v>35.405922451983479</v>
       </c>
       <c r="D50">
-        <v>117.4538352272727</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>7.475537552038396</v>
+        <v>7.4755375520383964</v>
       </c>
       <c r="B51">
-        <v>32.32857805365403</v>
+        <v>32.32857805140069</v>
       </c>
       <c r="C51">
-        <v>38.55847015657253</v>
+        <v>38.557239528665093</v>
       </c>
       <c r="D51">
         <v>151.9990808823529</v>
@@ -1233,15 +1265,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>6.416061702972498</v>
+        <v>6.4160617029725016</v>
       </c>
       <c r="B52">
-        <v>25.77629030620385</v>
+        <v>25.776290304986318</v>
       </c>
       <c r="C52">
-        <v>33.03120032481272</v>
+        <v>33.03652541144546</v>
       </c>
       <c r="D52">
         <v>129.19921875</v>
@@ -1250,32 +1282,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>6.855804335767697</v>
+        <v>6.8558043357713316</v>
       </c>
       <c r="B53">
-        <v>23.81158242907151</v>
+        <v>23.811582427088929</v>
       </c>
       <c r="C53">
-        <v>33.00654159278431</v>
+        <v>33.012258963470622</v>
       </c>
       <c r="D53">
-        <v>117.4538352272727</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>7.255129143419145</v>
+        <v>7.2551291434193734</v>
       </c>
       <c r="B54">
-        <v>18.92218187826009</v>
+        <v>18.922181876889919</v>
       </c>
       <c r="C54">
-        <v>34.41939752992906</v>
+        <v>34.421107621114928</v>
       </c>
       <c r="D54">
         <v>151.9990808823529</v>
@@ -1284,15 +1316,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5.164684490510194</v>
+        <v>5.1646844904520428</v>
       </c>
       <c r="B55">
-        <v>22.18374224363556</v>
+        <v>22.183742242665168</v>
       </c>
       <c r="C55">
-        <v>37.99215618001896</v>
+        <v>37.980278169450372</v>
       </c>
       <c r="D55">
         <v>143.5546875</v>
@@ -1301,15 +1333,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>4.489283414802704</v>
+        <v>4.4892834148099734</v>
       </c>
       <c r="B56">
-        <v>19.50041873367441</v>
+        <v>19.500418732885741</v>
       </c>
       <c r="C56">
-        <v>33.91418252643266</v>
+        <v>33.897814076603701</v>
       </c>
       <c r="D56">
         <v>172.265625</v>
@@ -1318,15 +1350,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>6.637761262953299</v>
+        <v>6.6377612629534131</v>
       </c>
       <c r="B57">
-        <v>29.94738745198287</v>
+        <v>29.947387450005738</v>
       </c>
       <c r="C57">
-        <v>41.43519435941819</v>
+        <v>41.440755719398297</v>
       </c>
       <c r="D57">
         <v>143.5546875</v>
@@ -1335,15 +1367,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>14.99978134577416</v>
       </c>
       <c r="B58">
-        <v>39.58036297016935</v>
+        <v>39.580362963422033</v>
       </c>
       <c r="C58">
-        <v>46.31831565577998</v>
+        <v>46.321716271358582</v>
       </c>
       <c r="D58">
         <v>103.359375</v>
@@ -1352,49 +1384,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4.437692449492137</v>
       </c>
       <c r="B59">
-        <v>21.16967936541061</v>
+        <v>21.169679362928289</v>
       </c>
       <c r="C59">
-        <v>44.43777208687523</v>
+        <v>44.425417890807473</v>
       </c>
       <c r="D59">
-        <v>135.999177631579</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>3.900149934525434</v>
+        <v>3.900149934525547</v>
       </c>
       <c r="B60">
-        <v>7.323241487406045</v>
+        <v>7.3232414870607743</v>
       </c>
       <c r="C60">
-        <v>37.99784806279082</v>
+        <v>38.003076412401882</v>
       </c>
       <c r="D60">
-        <v>89.10290948275862</v>
+        <v>89.102909482758619</v>
       </c>
       <c r="E60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>7.277391978475455</v>
       </c>
       <c r="B61">
-        <v>28.21012770629961</v>
+        <v>28.210127703077681</v>
       </c>
       <c r="C61">
-        <v>43.11542972189567</v>
+        <v>43.127577980244517</v>
       </c>
       <c r="D61">
         <v>161.4990234375</v>
@@ -1403,15 +1435,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3.09924912193032</v>
       </c>
       <c r="B62">
-        <v>15.00188023171462</v>
+        <v>15.00188022922867</v>
       </c>
       <c r="C62">
-        <v>42.92713889513669</v>
+        <v>42.917503854856363</v>
       </c>
       <c r="D62">
         <v>143.5546875</v>
@@ -1420,15 +1452,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2.945462729168419</v>
       </c>
       <c r="B63">
-        <v>12.48232129482978</v>
+        <v>12.482321293274239</v>
       </c>
       <c r="C63">
-        <v>38.49115961742779</v>
+        <v>38.476925523001547</v>
       </c>
       <c r="D63">
         <v>172.265625</v>
@@ -1437,15 +1469,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>7.431046371835503</v>
+        <v>7.4310463718355031</v>
       </c>
       <c r="B64">
-        <v>26.51755124686898</v>
+        <v>26.517551243786979</v>
       </c>
       <c r="C64">
-        <v>37.92566322657804</v>
+        <v>37.914076430220021</v>
       </c>
       <c r="D64">
         <v>161.4990234375</v>
@@ -1454,15 +1486,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2.810516925935536</v>
       </c>
       <c r="B65">
-        <v>12.04410119139775</v>
+        <v>12.044101190269711</v>
       </c>
       <c r="C65">
-        <v>35.93511706233521</v>
+        <v>35.930706477947169</v>
       </c>
       <c r="D65">
         <v>258.3984375</v>
@@ -1471,15 +1503,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3.09438440177604</v>
+        <v>3.0943844017751312</v>
       </c>
       <c r="B66">
-        <v>11.88476385190416</v>
+        <v>11.88476384848779</v>
       </c>
       <c r="C66">
-        <v>34.9861876850733</v>
+        <v>34.980884889967783</v>
       </c>
       <c r="D66">
         <v>143.5546875</v>
@@ -1488,15 +1520,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>2.662372372240395</v>
+        <v>2.6623723722403949</v>
       </c>
       <c r="B67">
-        <v>9.814044981872495</v>
+        <v>9.8140449805531986</v>
       </c>
       <c r="C67">
-        <v>37.01059156781837</v>
+        <v>37.002665569007007</v>
       </c>
       <c r="D67">
         <v>234.9076704545455</v>
@@ -1505,15 +1537,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>6.201783608219563</v>
+        <v>6.2017836082195634</v>
       </c>
       <c r="B68">
-        <v>22.150681577738</v>
+        <v>22.15068157550828</v>
       </c>
       <c r="C68">
-        <v>33.87040268880774</v>
+        <v>33.868750721791507</v>
       </c>
       <c r="D68">
         <v>184.5703125</v>
@@ -1522,32 +1554,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>6.074222039426552</v>
+        <v>6.0742220394265516</v>
       </c>
       <c r="B69">
-        <v>23.49599745470832</v>
+        <v>23.495997452731189</v>
       </c>
       <c r="C69">
-        <v>34.38793566525091</v>
+        <v>34.392340109396358</v>
       </c>
       <c r="D69">
-        <v>135.999177631579</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E69">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>2.82618506675233</v>
+        <v>2.8261850667523301</v>
       </c>
       <c r="B70">
-        <v>10.69650476944243</v>
+        <v>10.696504768214</v>
       </c>
       <c r="C70">
-        <v>41.44091913719519</v>
+        <v>41.443556269900348</v>
       </c>
       <c r="D70">
         <v>172.265625</v>
@@ -1556,32 +1588,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>5.445903340180529</v>
+        <v>5.4459033401805286</v>
       </c>
       <c r="B71">
-        <v>23.87893623722562</v>
+        <v>23.878936235811828</v>
       </c>
       <c r="C71">
-        <v>37.5650518549415</v>
+        <v>37.556639550467636</v>
       </c>
       <c r="D71">
-        <v>198.7680288461538</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>4.929571226429352</v>
+        <v>4.9295712264293519</v>
       </c>
       <c r="B72">
-        <v>18.86216493043444</v>
+        <v>18.86216492886436</v>
       </c>
       <c r="C72">
-        <v>31.98737285794479</v>
+        <v>31.94648746873025</v>
       </c>
       <c r="D72">
         <v>92.28515625</v>
@@ -1590,15 +1622,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>4.182327875454178</v>
+        <v>4.1823278754505431</v>
       </c>
       <c r="B73">
-        <v>13.25928516237412</v>
+        <v>13.25928516135648</v>
       </c>
       <c r="C73">
-        <v>29.42661020535848</v>
+        <v>29.42007298948641</v>
       </c>
       <c r="D73">
         <v>184.5703125</v>
@@ -1607,32 +1639,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>4.195973852724425</v>
+        <v>4.1959738527244248</v>
       </c>
       <c r="B74">
-        <v>18.58962116708111</v>
+        <v>18.589621165518309</v>
       </c>
       <c r="C74">
-        <v>33.51850354886712</v>
+        <v>33.517513802980638</v>
       </c>
       <c r="D74">
-        <v>135.999177631579</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3.487893461521459</v>
       </c>
       <c r="B75">
-        <v>17.32270181958818</v>
+        <v>17.322701819057549</v>
       </c>
       <c r="C75">
-        <v>31.3898091648683</v>
+        <v>31.391737829844519</v>
       </c>
       <c r="D75">
         <v>143.5546875</v>
@@ -1641,15 +1673,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>5.240361055312785</v>
+        <v>5.2403610553127846</v>
       </c>
       <c r="B76">
-        <v>17.996925772492</v>
+        <v>17.996925769162409</v>
       </c>
       <c r="C76">
-        <v>29.95326882979872</v>
+        <v>29.949423406457239</v>
       </c>
       <c r="D76">
         <v>123.046875</v>
@@ -1658,15 +1690,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>5.201713067217266</v>
+        <v>5.2017130672172662</v>
       </c>
       <c r="B77">
-        <v>18.25768309186477</v>
+        <v>18.257683089128051</v>
       </c>
       <c r="C77">
-        <v>32.47883366780005</v>
+        <v>32.479267181390298</v>
       </c>
       <c r="D77">
         <v>129.19921875</v>
@@ -1675,15 +1707,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>2.918214383400706</v>
+        <v>2.9182143834007062</v>
       </c>
       <c r="B78">
-        <v>13.65734720949142</v>
+        <v>13.657347208183021</v>
       </c>
       <c r="C78">
-        <v>42.06468135485986</v>
+        <v>42.074039071318538</v>
       </c>
       <c r="D78">
         <v>161.4990234375</v>
@@ -1692,15 +1724,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3.65949502856506</v>
+        <v>3.6594950285650598</v>
       </c>
       <c r="B79">
-        <v>20.01934703001486</v>
+        <v>20.019347028898181</v>
       </c>
       <c r="C79">
-        <v>35.97037204978675</v>
+        <v>35.963371476734658</v>
       </c>
       <c r="D79">
         <v>92.28515625</v>
@@ -1709,15 +1741,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>3.294949505710156</v>
+        <v>3.2949495057101559</v>
       </c>
       <c r="B80">
-        <v>16.15565490640025</v>
+        <v>16.15565490474296</v>
       </c>
       <c r="C80">
-        <v>36.50506163115602</v>
+        <v>36.494148416749681</v>
       </c>
       <c r="D80">
         <v>184.5703125</v>
@@ -1726,15 +1758,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>3.264764456886296</v>
+        <v>3.2647644568862959</v>
       </c>
       <c r="B81">
-        <v>14.22669275575065</v>
+        <v>14.226692754578099</v>
       </c>
       <c r="C81">
-        <v>41.50043284606551</v>
+        <v>41.496910460179009</v>
       </c>
       <c r="D81">
         <v>107.666015625</v>
@@ -1743,15 +1775,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>7.243747617968297</v>
+        <v>7.2437476179692064</v>
       </c>
       <c r="B82">
-        <v>22.52579910333943</v>
+        <v>22.525799102468081</v>
       </c>
       <c r="C82">
-        <v>36.49919487508554</v>
+        <v>36.501035112347417</v>
       </c>
       <c r="D82">
         <v>151.9990808823529</v>
@@ -1760,15 +1792,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>3.954620987279101</v>
+        <v>3.9546209872936098</v>
       </c>
       <c r="B83">
-        <v>13.02433326260586</v>
+        <v>13.024333261232499</v>
       </c>
       <c r="C83">
-        <v>29.93873551502285</v>
+        <v>29.934003231878268</v>
       </c>
       <c r="D83">
         <v>151.9990808823529</v>
@@ -1777,15 +1809,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>3.940728188157676</v>
+        <v>3.94072818815813</v>
       </c>
       <c r="B84">
-        <v>16.33634639927842</v>
+        <v>16.336346397177721</v>
       </c>
       <c r="C84">
-        <v>35.48953893002296</v>
+        <v>35.468156552300393</v>
       </c>
       <c r="D84">
         <v>151.9990808823529</v>
@@ -1794,15 +1826,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>5.597159111420137</v>
+        <v>5.5971591114201367</v>
       </c>
       <c r="B85">
-        <v>23.22546376937725</v>
+        <v>23.225463767527319</v>
       </c>
       <c r="C85">
-        <v>34.93428671935403</v>
+        <v>34.932298305169688</v>
       </c>
       <c r="D85">
         <v>151.9990808823529</v>
@@ -1811,32 +1843,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>5.626907092002805</v>
+        <v>5.6269070920028046</v>
       </c>
       <c r="B86">
-        <v>24.2969857182944</v>
+        <v>24.29698571631182</v>
       </c>
       <c r="C86">
-        <v>36.00326357837083</v>
+        <v>36.001521314561607</v>
       </c>
       <c r="D86">
-        <v>135.999177631579</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>2.872349725029978</v>
+        <v>2.8723497250299781</v>
       </c>
       <c r="B87">
-        <v>10.06437830772857</v>
+        <v>10.064378306225279</v>
       </c>
       <c r="C87">
-        <v>33.00767784097746</v>
+        <v>33.007807974195487</v>
       </c>
       <c r="D87">
         <v>92.28515625</v>
@@ -1845,15 +1877,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>3.25343039230965</v>
+        <v>3.2534303923096499</v>
       </c>
       <c r="B88">
-        <v>12.49755402196561</v>
+        <v>12.49755402064268</v>
       </c>
       <c r="C88">
-        <v>36.96324569568694</v>
+        <v>36.968810758977483</v>
       </c>
       <c r="D88">
         <v>184.5703125</v>
@@ -1862,32 +1894,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>3.912705333783839</v>
+        <v>3.9127053337838391</v>
       </c>
       <c r="B89">
-        <v>18.49845791165375</v>
+        <v>18.498457910828279</v>
       </c>
       <c r="C89">
-        <v>38.03838961915061</v>
+        <v>38.030010219648616</v>
       </c>
       <c r="D89">
-        <v>112.3471467391304</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E89">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>3.795905484955807</v>
+        <v>3.7959054849558069</v>
       </c>
       <c r="B90">
-        <v>17.5912413726508</v>
+        <v>17.59124137070712</v>
       </c>
       <c r="C90">
-        <v>34.36711845046337</v>
+        <v>34.363961285594833</v>
       </c>
       <c r="D90">
         <v>215.33203125</v>
@@ -1896,32 +1928,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>7.383803066232351</v>
+        <v>7.3838030662323506</v>
       </c>
       <c r="B91">
-        <v>27.29515599792777</v>
+        <v>27.29515599510745</v>
       </c>
       <c r="C91">
-        <v>39.03932727517562</v>
+        <v>39.038943397243251</v>
       </c>
       <c r="D91">
-        <v>117.4538352272727</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>7.204485301010041</v>
+        <v>7.2044853010100409</v>
       </c>
       <c r="B92">
-        <v>25.87775740803184</v>
+        <v>25.877757403021779</v>
       </c>
       <c r="C92">
-        <v>38.49099951938531</v>
+        <v>38.498970279531967</v>
       </c>
       <c r="D92">
         <v>151.9990808823529</v>
@@ -1930,15 +1962,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>5.310133280034684</v>
+        <v>5.3101332800346839</v>
       </c>
       <c r="B93">
-        <v>24.21075366736222</v>
+        <v>24.210753664919881</v>
       </c>
       <c r="C93">
-        <v>42.02434354407257</v>
+        <v>42.027331717943639</v>
       </c>
       <c r="D93">
         <v>143.5546875</v>
@@ -1947,15 +1979,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>6.573123796321354</v>
+        <v>6.5731237961759756</v>
       </c>
       <c r="B94">
-        <v>27.48008041887693</v>
+        <v>27.480080416714451</v>
       </c>
       <c r="C94">
-        <v>42.09493735010603</v>
+        <v>42.086367523159851</v>
       </c>
       <c r="D94">
         <v>161.4990234375</v>
@@ -1964,32 +1996,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>3.211257583430918</v>
+        <v>3.2112575834309181</v>
       </c>
       <c r="B95">
-        <v>12.58568583434664</v>
+        <v>12.58568583176802</v>
       </c>
       <c r="C95">
-        <v>38.43578361810775</v>
+        <v>38.435627934232393</v>
       </c>
       <c r="D95">
-        <v>198.7680288461538</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E95">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>9.289180898782138</v>
+        <v>9.2891808987821385</v>
       </c>
       <c r="B96">
-        <v>29.39952009469993</v>
+        <v>29.399520091814189</v>
       </c>
       <c r="C96">
-        <v>38.47826228506094</v>
+        <v>38.477170520338447</v>
       </c>
       <c r="D96">
         <v>123.046875</v>
@@ -1998,15 +2030,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>3.997621300576199</v>
+        <v>3.99762130063435</v>
       </c>
       <c r="B97">
-        <v>19.22682677173204</v>
+        <v>19.226826771681161</v>
       </c>
       <c r="C97">
-        <v>38.95655842189725</v>
+        <v>38.95866244677935</v>
       </c>
       <c r="D97">
         <v>184.5703125</v>
@@ -2015,15 +2047,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>6.160293708687748</v>
+        <v>6.1602937086877478</v>
       </c>
       <c r="B98">
-        <v>21.60013550855953</v>
+        <v>21.600135507034889</v>
       </c>
       <c r="C98">
-        <v>33.94420188369679</v>
+        <v>33.935268214335167</v>
       </c>
       <c r="D98">
         <v>172.265625</v>
@@ -2032,15 +2064,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>4.60148611049233</v>
+        <v>4.6014861104923304</v>
       </c>
       <c r="B99">
-        <v>23.05211134166971</v>
+        <v>23.0521113403763</v>
       </c>
       <c r="C99">
-        <v>37.89695124741111</v>
+        <v>37.884638595079878</v>
       </c>
       <c r="D99">
         <v>172.265625</v>
@@ -2049,15 +2081,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>2.677279307522215</v>
+        <v>2.6772793075222152</v>
       </c>
       <c r="B100">
-        <v>11.16689692463453</v>
+        <v>11.16689692271737</v>
       </c>
       <c r="C100">
-        <v>36.46256672350459</v>
+        <v>36.47428110608633</v>
       </c>
       <c r="D100">
         <v>143.5546875</v>
@@ -2066,32 +2098,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>4.909413883037121</v>
+        <v>4.9094138830371206</v>
       </c>
       <c r="B101">
-        <v>19.69972150125765</v>
+        <v>19.699721500821521</v>
       </c>
       <c r="C101">
-        <v>34.01937852882617</v>
+        <v>34.016324322690608</v>
       </c>
       <c r="D101">
-        <v>112.3471467391304</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E101">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>5.889655879363604</v>
+        <v>5.8896558793636036</v>
       </c>
       <c r="B102">
-        <v>22.72578539799812</v>
+        <v>22.725785395108741</v>
       </c>
       <c r="C102">
-        <v>33.90069763295269</v>
+        <v>33.892039064125093</v>
       </c>
       <c r="D102">
         <v>129.19921875</v>
@@ -2100,15 +2132,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>4.069711964158315</v>
+        <v>4.0697119641583148</v>
       </c>
       <c r="B103">
-        <v>23.86647641762122</v>
+        <v>23.866476415880321</v>
       </c>
       <c r="C103">
-        <v>41.47362701765094</v>
+        <v>41.46550028367222</v>
       </c>
       <c r="D103">
         <v>71.77734375</v>
@@ -2117,15 +2149,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>3.841954837862576</v>
+        <v>3.8419548378625761</v>
       </c>
       <c r="B104">
-        <v>19.49595163479773</v>
+        <v>19.495951632535299</v>
       </c>
       <c r="C104">
-        <v>42.93595406378882</v>
+        <v>42.936803935067928</v>
       </c>
       <c r="D104">
         <v>95.703125</v>
@@ -2134,15 +2166,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>3.119679772105312</v>
+        <v>3.1196797721053122</v>
       </c>
       <c r="B105">
-        <v>14.95685782784629</v>
+        <v>14.956857826516091</v>
       </c>
       <c r="C105">
-        <v>41.04205990232524</v>
+        <v>41.047400006195453</v>
       </c>
       <c r="D105">
         <v>161.4990234375</v>
@@ -2151,32 +2183,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>3.267504720737752</v>
+        <v>3.2675047207450212</v>
       </c>
       <c r="B106">
-        <v>12.87500207319321</v>
+        <v>12.875002072191251</v>
       </c>
       <c r="C106">
-        <v>38.47850581368616</v>
+        <v>38.45829434146647</v>
       </c>
       <c r="D106">
-        <v>112.3471467391304</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E106">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>5.457773218705063</v>
+        <v>5.4577732187050634</v>
       </c>
       <c r="B107">
-        <v>22.68520546230855</v>
+        <v>22.685205460569481</v>
       </c>
       <c r="C107">
-        <v>34.98244229023738</v>
+        <v>34.968029209973068</v>
       </c>
       <c r="D107">
         <v>143.5546875</v>
@@ -2185,49 +2217,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>2.829572719917795</v>
+        <v>2.8295727199177949</v>
       </c>
       <c r="B108">
-        <v>12.59001526463703</v>
+        <v>12.59001526166452</v>
       </c>
       <c r="C108">
-        <v>42.9864865482425</v>
+        <v>42.980796973193307</v>
       </c>
       <c r="D108">
-        <v>117.4538352272727</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E108">
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>3.619380328577904</v>
+        <v>3.619380328585172</v>
       </c>
       <c r="B109">
-        <v>16.50796282760399</v>
+        <v>16.507962825546901</v>
       </c>
       <c r="C109">
-        <v>38.59784391781841</v>
+        <v>38.592060599761943</v>
       </c>
       <c r="D109">
-        <v>135.999177631579</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E109">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>3.556404679844902</v>
+        <v>3.5564046798449018</v>
       </c>
       <c r="B110">
-        <v>15.9484781819461</v>
+        <v>15.94847817942926</v>
       </c>
       <c r="C110">
-        <v>39.93055743455468</v>
+        <v>39.915097560588983</v>
       </c>
       <c r="D110">
         <v>161.4990234375</v>
@@ -2236,15 +2268,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>8.210754720669071</v>
+        <v>8.2107547206690707</v>
       </c>
       <c r="B111">
-        <v>24.12822157032684</v>
+        <v>24.12822156405382</v>
       </c>
       <c r="C111">
-        <v>40.98140314119281</v>
+        <v>40.987858632834808</v>
       </c>
       <c r="D111">
         <v>123.046875</v>
@@ -2253,15 +2285,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>4.334794326870016</v>
+        <v>4.3347943268990914</v>
       </c>
       <c r="B112">
-        <v>21.44988729512558</v>
+        <v>21.449887292690519</v>
       </c>
       <c r="C112">
-        <v>41.93762958969138</v>
+        <v>41.921301275975082</v>
       </c>
       <c r="D112">
         <v>64.599609375</v>
@@ -2270,15 +2302,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>3.295597909787278</v>
+        <v>3.2955979097872778</v>
       </c>
       <c r="B113">
-        <v>15.35451264099576</v>
+        <v>15.354512639825471</v>
       </c>
       <c r="C113">
-        <v>41.413061011413</v>
+        <v>41.412450990211987</v>
       </c>
       <c r="D113">
         <v>184.5703125</v>
@@ -2287,15 +2319,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>7.722223345030803</v>
+        <v>7.7222233450308027</v>
       </c>
       <c r="B114">
-        <v>31.48890596420191</v>
+        <v>31.488905961585228</v>
       </c>
       <c r="C114">
-        <v>39.9998537641947</v>
+        <v>39.996084994565827</v>
       </c>
       <c r="D114">
         <v>151.9990808823529</v>
@@ -2304,20 +2336,666 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>3.090768696856278</v>
+        <v>3.0907686968562782</v>
       </c>
       <c r="B115">
-        <v>14.82635870514327</v>
+        <v>14.82635870255192</v>
       </c>
       <c r="C115">
-        <v>40.98506824144622</v>
+        <v>40.9764986705461</v>
       </c>
       <c r="D115">
         <v>172.265625</v>
       </c>
       <c r="E115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>4.3243824623552696</v>
+      </c>
+      <c r="B116">
+        <v>17.329834019276269</v>
+      </c>
+      <c r="C116">
+        <v>34.003807962942879</v>
+      </c>
+      <c r="D116">
+        <v>129.19921875</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>15.496612233279439</v>
+      </c>
+      <c r="B117">
+        <v>28.717579212558601</v>
+      </c>
+      <c r="C117">
+        <v>38.563911143791962</v>
+      </c>
+      <c r="D117">
+        <v>107.666015625</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>9.2782395059153391</v>
+      </c>
+      <c r="B118">
+        <v>31.829373132907349</v>
+      </c>
+      <c r="C118">
+        <v>44.548041992063332</v>
+      </c>
+      <c r="D118">
+        <v>123.046875</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>17.643585613099479</v>
+      </c>
+      <c r="B119">
+        <v>47.196543721446879</v>
+      </c>
+      <c r="C119">
+        <v>58.593006567006611</v>
+      </c>
+      <c r="D119">
+        <v>129.19921875</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>5.4802969582351251</v>
+      </c>
+      <c r="B120">
+        <v>18.22549514458359</v>
+      </c>
+      <c r="C120">
+        <v>37.903137783356136</v>
+      </c>
+      <c r="D120">
+        <v>107.666015625</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>11.87667611929561</v>
+      </c>
+      <c r="B121">
+        <v>28.87969313765354</v>
+      </c>
+      <c r="C121">
+        <v>44.011277749323092</v>
+      </c>
+      <c r="D121">
+        <v>86.1328125</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>24.30955290803595</v>
+      </c>
+      <c r="B122">
+        <v>51.229449548884041</v>
+      </c>
+      <c r="C122">
+        <v>74.583457444190088</v>
+      </c>
+      <c r="D122">
+        <v>117.45383522727271</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>18.608445942296299</v>
+      </c>
+      <c r="B123">
+        <v>39.453034853176931</v>
+      </c>
+      <c r="C123">
+        <v>39.499360121115828</v>
+      </c>
+      <c r="D123">
+        <v>129.19921875</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>11.43501010074778</v>
+      </c>
+      <c r="B124">
+        <v>20.097487750556802</v>
+      </c>
+      <c r="C124">
+        <v>31.983511474034621</v>
+      </c>
+      <c r="D124">
+        <v>129.19921875</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>9.0956236561017008</v>
+      </c>
+      <c r="B125">
+        <v>30.536121939665499</v>
+      </c>
+      <c r="C125">
+        <v>38.563172632784642</v>
+      </c>
+      <c r="D125">
+        <v>172.265625</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>6.2626992706517379</v>
+      </c>
+      <c r="B126">
+        <v>21.081622695127869</v>
+      </c>
+      <c r="C126">
+        <v>35.447868406241497</v>
+      </c>
+      <c r="D126">
+        <v>123.046875</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>11.57915143547722</v>
+      </c>
+      <c r="B127">
+        <v>19.818365200808671</v>
+      </c>
+      <c r="C127">
+        <v>28.533322907590762</v>
+      </c>
+      <c r="D127">
+        <v>129.19921875</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>8.2871666985000214</v>
+      </c>
+      <c r="B128">
+        <v>21.25169668774997</v>
+      </c>
+      <c r="C128">
+        <v>29.116207042437029</v>
+      </c>
+      <c r="D128">
+        <v>112.34714673913039</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>12.141897784218539</v>
+      </c>
+      <c r="B129">
+        <v>27.601770668666632</v>
+      </c>
+      <c r="C129">
+        <v>28.53322250024107</v>
+      </c>
+      <c r="D129">
+        <v>123.046875</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>7.0566664626353948</v>
+      </c>
+      <c r="B130">
+        <v>20.50148910291761</v>
+      </c>
+      <c r="C130">
+        <v>24.016621854182439</v>
+      </c>
+      <c r="D130">
+        <v>135.99917763157899</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>6.6089268378391104</v>
+      </c>
+      <c r="B131">
+        <v>21.881208476677621</v>
+      </c>
+      <c r="C131">
+        <v>25.47330956688867</v>
+      </c>
+      <c r="D131">
+        <v>151.9990808823529</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>13.08082458471026</v>
+      </c>
+      <c r="B132">
+        <v>20.458707810205549</v>
+      </c>
+      <c r="C132">
+        <v>27.055665953878311</v>
+      </c>
+      <c r="D132">
+        <v>135.99917763157899</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>11.92941465193708</v>
+      </c>
+      <c r="B133">
+        <v>21.34228840236667</v>
+      </c>
+      <c r="C133">
+        <v>27.952445402614948</v>
+      </c>
+      <c r="D133">
+        <v>151.9990808823529</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>4.8927031714092291</v>
+      </c>
+      <c r="B134">
+        <v>23.81332129044219</v>
+      </c>
+      <c r="C134">
+        <v>42.509004627392891</v>
+      </c>
+      <c r="D134">
+        <v>123.046875</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>3.4114119729145251</v>
+      </c>
+      <c r="B135">
+        <v>13.489751573637079</v>
+      </c>
+      <c r="C135">
+        <v>39.447300475304459</v>
+      </c>
+      <c r="D135">
+        <v>103.359375</v>
+      </c>
+      <c r="E135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>6.5624261916615838</v>
+      </c>
+      <c r="B136">
+        <v>27.363720693581911</v>
+      </c>
+      <c r="C136">
+        <v>42.989934330996</v>
+      </c>
+      <c r="D136">
+        <v>135.99917763157899</v>
+      </c>
+      <c r="E136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>21.412058690460949</v>
+      </c>
+      <c r="B137">
+        <v>57.82901398006387</v>
+      </c>
+      <c r="C137">
+        <v>67.057395400158072</v>
+      </c>
+      <c r="D137">
+        <v>129.19921875</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>25.59963862647432</v>
+      </c>
+      <c r="B138">
+        <v>74.467206134096088</v>
+      </c>
+      <c r="C138">
+        <v>71.002974822139194</v>
+      </c>
+      <c r="D138">
+        <v>135.99917763157899</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>11.28985472001454</v>
+      </c>
+      <c r="B139">
+        <v>57.577889392898221</v>
+      </c>
+      <c r="C139">
+        <v>79.428552300596081</v>
+      </c>
+      <c r="D139">
+        <v>198.76802884615381</v>
+      </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>18.43958696364691</v>
+      </c>
+      <c r="B140">
+        <v>53.634536188248312</v>
+      </c>
+      <c r="C140">
+        <v>51.999174694914409</v>
+      </c>
+      <c r="D140">
+        <v>151.9990808823529</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>14.3965522465554</v>
+      </c>
+      <c r="B141">
+        <v>45.235221089484341</v>
+      </c>
+      <c r="C141">
+        <v>46.50779187352628</v>
+      </c>
+      <c r="D141">
+        <v>143.5546875</v>
+      </c>
+      <c r="E141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>27.709373913091909</v>
+      </c>
+      <c r="B142">
+        <v>65.752106619572231</v>
+      </c>
+      <c r="C142">
+        <v>56.423163316461881</v>
+      </c>
+      <c r="D142">
+        <v>123.046875</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>9.2706406141015378</v>
+      </c>
+      <c r="B143">
+        <v>28.126529384535271</v>
+      </c>
+      <c r="C143">
+        <v>40.976291963168961</v>
+      </c>
+      <c r="D143">
+        <v>184.5703125</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>16.51834679383802</v>
+      </c>
+      <c r="B144">
+        <v>37.376722805629598</v>
+      </c>
+      <c r="C144">
+        <v>45.633330635677432</v>
+      </c>
+      <c r="D144">
+        <v>129.19921875</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>9.4928905094418568</v>
+      </c>
+      <c r="B145">
+        <v>23.05129324263833</v>
+      </c>
+      <c r="C145">
+        <v>33.923142957970107</v>
+      </c>
+      <c r="D145">
+        <v>103.359375</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>12.224263835217609</v>
+      </c>
+      <c r="B146">
+        <v>25.71383238698342</v>
+      </c>
+      <c r="C146">
+        <v>32.970551666702782</v>
+      </c>
+      <c r="D146">
+        <v>151.9990808823529</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>9.8372824835755033</v>
+      </c>
+      <c r="B147">
+        <v>20.617251667576291</v>
+      </c>
+      <c r="C147">
+        <v>23.97511301585428</v>
+      </c>
+      <c r="D147">
+        <v>161.4990234375</v>
+      </c>
+      <c r="E147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>7.5198120824071637</v>
+      </c>
+      <c r="B148">
+        <v>21.23877946737802</v>
+      </c>
+      <c r="C148">
+        <v>23.023096355926249</v>
+      </c>
+      <c r="D148">
+        <v>117.45383522727271</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>10.16534746441871</v>
+      </c>
+      <c r="B149">
+        <v>19.672904454870011</v>
+      </c>
+      <c r="C149">
+        <v>22.00061525760561</v>
+      </c>
+      <c r="D149">
+        <v>112.34714673913039</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>8.5904837391892457</v>
+      </c>
+      <c r="B150">
+        <v>22.67185656653098</v>
+      </c>
+      <c r="C150">
+        <v>22.98710423966865</v>
+      </c>
+      <c r="D150">
+        <v>161.4990234375</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>7.2988340137923746</v>
+      </c>
+      <c r="B151">
+        <v>17.984033903783661</v>
+      </c>
+      <c r="C151">
+        <v>23.013595584347769</v>
+      </c>
+      <c r="D151">
+        <v>198.76802884615381</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>6.1022749135762933</v>
+      </c>
+      <c r="B152">
+        <v>16.755355871137521</v>
+      </c>
+      <c r="C152">
+        <v>22.990994866392501</v>
+      </c>
+      <c r="D152">
+        <v>184.5703125</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>6.5381672796546173</v>
+      </c>
+      <c r="B153">
+        <v>16.69327069603257</v>
+      </c>
+      <c r="C153">
+        <v>23.983222805788991</v>
+      </c>
+      <c r="D153">
+        <v>161.4990234375</v>
+      </c>
+      <c r="E153">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ANN Model deployed and accuracy measured
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saswat\Desktop\KnockMLDatasetGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DC1259-5EFB-489F-9077-14BB6C74DCFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A784865-45A5-4486-9608-05F2BDC55C13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -393,23 +400,23 @@
   <dimension ref="A1:E153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>12.207933978758341</v>
+        <v>13.08082458471026</v>
       </c>
       <c r="B1">
-        <v>31.158824221723918</v>
+        <v>20.458707810205549</v>
       </c>
       <c r="C1">
-        <v>43.486968097800784</v>
+        <v>27.055665953878311</v>
       </c>
       <c r="D1">
-        <v>161.4990234375</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E1">
         <v>0</v>
@@ -417,16 +424,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>9.0272165811578589</v>
+        <v>18.608445942296299</v>
       </c>
       <c r="B2">
-        <v>27.381006255621902</v>
+        <v>39.453034853176931</v>
       </c>
       <c r="C2">
-        <v>42.523310884066412</v>
+        <v>39.499360121115828</v>
       </c>
       <c r="D2">
-        <v>112.34714673913039</v>
+        <v>129.19921875</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -434,67 +441,67 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>11.080650933467711</v>
+        <v>7.3838030662323506</v>
       </c>
       <c r="B3">
-        <v>29.76354408711169</v>
+        <v>27.29515599510745</v>
       </c>
       <c r="C3">
-        <v>40.963686312294342</v>
+        <v>39.038943397243251</v>
       </c>
       <c r="D3">
-        <v>198.76802884615381</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>16.68356557880529</v>
+        <v>3.8419548378625761</v>
       </c>
       <c r="B4">
-        <v>41.620958322188947</v>
+        <v>19.495951632535299</v>
       </c>
       <c r="C4">
-        <v>48.985580429468172</v>
+        <v>42.936803935067928</v>
       </c>
       <c r="D4">
-        <v>161.4990234375</v>
+        <v>95.703125</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>16.7137039099755</v>
+        <v>2.810516925935536</v>
       </c>
       <c r="B5">
-        <v>36.852265219518692</v>
+        <v>12.044101190269711</v>
       </c>
       <c r="C5">
-        <v>50.915033584508578</v>
+        <v>35.930706477947169</v>
       </c>
       <c r="D5">
-        <v>151.9990808823529</v>
+        <v>258.3984375</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10.308673072178751</v>
+        <v>8.6317387085714046</v>
       </c>
       <c r="B6">
-        <v>28.850810959942969</v>
+        <v>36.132342807291593</v>
       </c>
       <c r="C6">
-        <v>49.885919312899837</v>
+        <v>36.961703901971923</v>
       </c>
       <c r="D6">
-        <v>103.359375</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -502,33 +509,33 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8.6105030850522262</v>
+        <v>7.2044853010100409</v>
       </c>
       <c r="B7">
-        <v>25.299262163450589</v>
+        <v>25.877757403021779</v>
       </c>
       <c r="C7">
-        <v>43.970209075691322</v>
+        <v>38.498970279531967</v>
       </c>
       <c r="D7">
-        <v>103.359375</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10.47633707116122</v>
+        <v>8.4267397088328568</v>
       </c>
       <c r="B8">
-        <v>27.097502847925739</v>
+        <v>25.232760662107658</v>
       </c>
       <c r="C8">
-        <v>39.370375152842463</v>
+        <v>36.5214782319091</v>
       </c>
       <c r="D8">
-        <v>129.19921875</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -536,16 +543,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11.38424189674268</v>
+        <v>7.7902616791126329</v>
       </c>
       <c r="B9">
-        <v>26.72121182224674</v>
+        <v>31.63863717845387</v>
       </c>
       <c r="C9">
-        <v>40.91013873046623</v>
+        <v>37.522729055934661</v>
       </c>
       <c r="D9">
-        <v>117.45383522727271</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -553,16 +560,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11.486211917823489</v>
+        <v>4.5626056587824264</v>
       </c>
       <c r="B10">
-        <v>34.62951404590715</v>
+        <v>17.338228218724161</v>
       </c>
       <c r="C10">
-        <v>48.069561029250607</v>
+        <v>28.927344406814139</v>
       </c>
       <c r="D10">
-        <v>143.5546875</v>
+        <v>103.359375</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -570,16 +577,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8.0087191789202343</v>
+        <v>4.4892834148099734</v>
       </c>
       <c r="B11">
-        <v>22.154053972843801</v>
+        <v>19.500418732885741</v>
       </c>
       <c r="C11">
-        <v>32.4665903079419</v>
+        <v>33.897814076603701</v>
       </c>
       <c r="D11">
-        <v>151.9990808823529</v>
+        <v>172.265625</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -587,16 +594,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5.3197985941934061</v>
+        <v>24.30955290803595</v>
       </c>
       <c r="B12">
-        <v>16.544426321543678</v>
+        <v>51.229449548884041</v>
       </c>
       <c r="C12">
-        <v>28.40577999519401</v>
+        <v>74.583457444190088</v>
       </c>
       <c r="D12">
-        <v>143.5546875</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -604,33 +611,33 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6.4157600748220611</v>
+        <v>6.1602937086877478</v>
       </c>
       <c r="B13">
-        <v>20.291186597306801</v>
+        <v>21.600135507034889</v>
       </c>
       <c r="C13">
-        <v>32.453595921390139</v>
+        <v>33.935268214335167</v>
       </c>
       <c r="D13">
-        <v>151.9990808823529</v>
+        <v>172.265625</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4.5626056587824264</v>
+        <v>6.4157600748220611</v>
       </c>
       <c r="B14">
-        <v>17.338228218724161</v>
+        <v>20.291186597306801</v>
       </c>
       <c r="C14">
-        <v>28.927344406814139</v>
+        <v>32.453595921390139</v>
       </c>
       <c r="D14">
-        <v>103.359375</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -638,16 +645,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>8.2361407722185547</v>
+        <v>8.0087191789202343</v>
       </c>
       <c r="B15">
-        <v>25.4386913714924</v>
+        <v>22.154053972843801</v>
       </c>
       <c r="C15">
-        <v>38.94734749929831</v>
+        <v>32.4665903079419</v>
       </c>
       <c r="D15">
-        <v>107.666015625</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -655,33 +662,33 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8.0217870655815702</v>
+        <v>2.945462729168419</v>
       </c>
       <c r="B16">
-        <v>22.947280559311029</v>
+        <v>12.482321293274239</v>
       </c>
       <c r="C16">
-        <v>38.458921919387009</v>
+        <v>38.476925523001547</v>
       </c>
       <c r="D16">
-        <v>151.9990808823529</v>
+        <v>172.265625</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>8.0450975918850762</v>
+        <v>8.2361407722185547</v>
       </c>
       <c r="B17">
-        <v>24.016997200347149</v>
+        <v>25.4386913714924</v>
       </c>
       <c r="C17">
-        <v>38.545769830713411</v>
+        <v>38.94734749929831</v>
       </c>
       <c r="D17">
-        <v>215.33203125</v>
+        <v>107.666015625</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -689,33 +696,33 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>7.6468955992826864</v>
+        <v>4.8927031714092291</v>
       </c>
       <c r="B18">
-        <v>22.34456281936933</v>
+        <v>23.81332129044219</v>
       </c>
       <c r="C18">
-        <v>34.462563191647519</v>
+        <v>42.509004627392891</v>
       </c>
       <c r="D18">
         <v>123.046875</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7.9018299084357686</v>
+        <v>9.2782395059153391</v>
       </c>
       <c r="B19">
-        <v>26.280142793695109</v>
+        <v>31.829373132907349</v>
       </c>
       <c r="C19">
-        <v>37.007836202058712</v>
+        <v>44.548041992063332</v>
       </c>
       <c r="D19">
-        <v>107.666015625</v>
+        <v>123.046875</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -723,13 +730,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5.8026525179051234</v>
+        <v>5.1646844904520428</v>
       </c>
       <c r="B20">
-        <v>25.75464201939657</v>
+        <v>22.183742242665168</v>
       </c>
       <c r="C20">
-        <v>36.948889560210567</v>
+        <v>37.980278169450372</v>
       </c>
       <c r="D20">
         <v>143.5546875</v>
@@ -740,30 +747,30 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9.3863607851169633</v>
+        <v>2.6772793075222152</v>
       </c>
       <c r="B21">
-        <v>30.05943567999979</v>
+        <v>11.16689692271737</v>
       </c>
       <c r="C21">
-        <v>42.485767903670506</v>
+        <v>36.47428110608633</v>
       </c>
       <c r="D21">
         <v>143.5546875</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7.0322616081352392</v>
+        <v>4.437692449492137</v>
       </c>
       <c r="B22">
-        <v>19.824700079752141</v>
+        <v>21.169679362928289</v>
       </c>
       <c r="C22">
-        <v>36.116781705269979</v>
+        <v>44.425417890807473</v>
       </c>
       <c r="D22">
         <v>135.99917763157899</v>
@@ -774,16 +781,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5.6070666806481224</v>
+        <v>8.0450975918850762</v>
       </c>
       <c r="B23">
-        <v>23.253547326020861</v>
+        <v>24.016997200347149</v>
       </c>
       <c r="C23">
-        <v>34.467388321699858</v>
+        <v>38.545769830713411</v>
       </c>
       <c r="D23">
-        <v>172.265625</v>
+        <v>215.33203125</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -791,33 +798,33 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>6.7123020916941467</v>
+        <v>3.0907686968562782</v>
       </c>
       <c r="B24">
-        <v>21.83760329880894</v>
+        <v>14.82635870255192</v>
       </c>
       <c r="C24">
-        <v>32.519685036464637</v>
+        <v>40.9764986705461</v>
       </c>
       <c r="D24">
-        <v>143.5546875</v>
+        <v>172.265625</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>10.435630621990329</v>
+        <v>5.9530824568297778</v>
       </c>
       <c r="B25">
-        <v>29.24294621450829</v>
+        <v>20.220915947519671</v>
       </c>
       <c r="C25">
-        <v>38.449738620713248</v>
+        <v>35.455778845739552</v>
       </c>
       <c r="D25">
-        <v>143.5546875</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -825,16 +832,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>7.9887799913592792</v>
+        <v>6.9158954991965906</v>
       </c>
       <c r="B26">
-        <v>22.287395115157938</v>
+        <v>30.32702352611448</v>
       </c>
       <c r="C26">
-        <v>32.938789923250873</v>
+        <v>37.924022565638808</v>
       </c>
       <c r="D26">
-        <v>151.9990808823529</v>
+        <v>73.828125</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -842,33 +849,33 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>6.092986008292697</v>
+        <v>2.8723497250299781</v>
       </c>
       <c r="B27">
-        <v>19.796859119338858</v>
+        <v>10.064378306225279</v>
       </c>
       <c r="C27">
-        <v>33.01676530885608</v>
+        <v>33.007807974195487</v>
       </c>
       <c r="D27">
-        <v>143.5546875</v>
+        <v>92.28515625</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>8.2618677271640983</v>
+        <v>6.8372574076607124</v>
       </c>
       <c r="B28">
-        <v>24.67375867885082</v>
+        <v>19.785642996173522</v>
       </c>
       <c r="C28">
-        <v>38.515744386381591</v>
+        <v>38.4927067156828</v>
       </c>
       <c r="D28">
-        <v>123.046875</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -876,50 +883,50 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>6.4730211748331614</v>
+        <v>4.6014861104923304</v>
       </c>
       <c r="B29">
-        <v>27.48818425779173</v>
+        <v>23.0521113403763</v>
       </c>
       <c r="C29">
-        <v>34.486773025201913</v>
+        <v>37.884638595079878</v>
       </c>
       <c r="D29">
-        <v>143.5546875</v>
+        <v>172.265625</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>6.4741871134093438</v>
+        <v>3.94072818815813</v>
       </c>
       <c r="B30">
-        <v>21.577448733102251</v>
+        <v>16.336346397177721</v>
       </c>
       <c r="C30">
-        <v>38.526859392719459</v>
+        <v>35.468156552300393</v>
       </c>
       <c r="D30">
         <v>151.9990808823529</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>5.9530824568297778</v>
+        <v>8.2871666985000214</v>
       </c>
       <c r="B31">
-        <v>20.220915947519671</v>
+        <v>21.25169668774997</v>
       </c>
       <c r="C31">
-        <v>35.455778845739552</v>
+        <v>29.116207042437029</v>
       </c>
       <c r="D31">
-        <v>161.4990234375</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -927,50 +934,50 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>6.0182590094305048</v>
+        <v>9.4928905094418568</v>
       </c>
       <c r="B32">
-        <v>17.699606603344741</v>
+        <v>23.05129324263833</v>
       </c>
       <c r="C32">
-        <v>32.464518842438899</v>
+        <v>33.923142957970107</v>
       </c>
       <c r="D32">
-        <v>143.5546875</v>
+        <v>103.359375</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>9.4420227619200858</v>
+        <v>5.4459033401805286</v>
       </c>
       <c r="B33">
-        <v>19.486697921961969</v>
+        <v>23.878936235811828</v>
       </c>
       <c r="C33">
-        <v>34.505199289614268</v>
+        <v>37.556639550467636</v>
       </c>
       <c r="D33">
-        <v>143.5546875</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3.7427248416158179</v>
+        <v>7.0322616081352392</v>
       </c>
       <c r="B34">
-        <v>12.107963297650761</v>
+        <v>19.824700079752141</v>
       </c>
       <c r="C34">
-        <v>33.964322679850817</v>
+        <v>36.116781705269979</v>
       </c>
       <c r="D34">
-        <v>143.5546875</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -978,50 +985,50 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>8.6317387085714046</v>
+        <v>16.51834679383802</v>
       </c>
       <c r="B35">
-        <v>36.132342807291593</v>
+        <v>37.376722805629598</v>
       </c>
       <c r="C35">
-        <v>36.961703901971923</v>
+        <v>45.633330635677432</v>
       </c>
       <c r="D35">
-        <v>151.9990808823529</v>
+        <v>129.19921875</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>9.2350463989826519</v>
+        <v>2.6623723722403949</v>
       </c>
       <c r="B36">
-        <v>28.751575764275319</v>
+        <v>9.8140449805531986</v>
       </c>
       <c r="C36">
-        <v>37.495795349310612</v>
+        <v>37.002665569007007</v>
       </c>
       <c r="D36">
-        <v>112.34714673913039</v>
+        <v>234.9076704545455</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>8.3301729425647597</v>
+        <v>11.38424189674268</v>
       </c>
       <c r="B37">
-        <v>32.137712447610951</v>
+        <v>26.72121182224674</v>
       </c>
       <c r="C37">
-        <v>50.001756461295628</v>
+        <v>40.91013873046623</v>
       </c>
       <c r="D37">
-        <v>143.5546875</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1029,16 +1036,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>6.9158954991965906</v>
+        <v>8.6105030850522262</v>
       </c>
       <c r="B38">
-        <v>30.32702352611448</v>
+        <v>25.299262163450589</v>
       </c>
       <c r="C38">
-        <v>37.924022565638808</v>
+        <v>43.970209075691322</v>
       </c>
       <c r="D38">
-        <v>73.828125</v>
+        <v>103.359375</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1046,16 +1053,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>6.092609462980052</v>
+        <v>11.57915143547722</v>
       </c>
       <c r="B39">
-        <v>20.34202310713675</v>
+        <v>19.818365200808671</v>
       </c>
       <c r="C39">
-        <v>34.443780104971822</v>
+        <v>28.533322907590762</v>
       </c>
       <c r="D39">
-        <v>123.046875</v>
+        <v>129.19921875</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1063,13 +1070,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>8.4267397088328568</v>
+        <v>6.6089268378391104</v>
       </c>
       <c r="B40">
-        <v>25.232760662107658</v>
+        <v>21.881208476677621</v>
       </c>
       <c r="C40">
-        <v>36.5214782319091</v>
+        <v>25.47330956688867</v>
       </c>
       <c r="D40">
         <v>151.9990808823529</v>
@@ -1080,67 +1087,67 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>5.492538208569048</v>
+        <v>3.2955979097872778</v>
       </c>
       <c r="B41">
-        <v>21.556054986619959</v>
+        <v>15.354512639825471</v>
       </c>
       <c r="C41">
-        <v>34.958524604244381</v>
+        <v>41.412450990211987</v>
       </c>
       <c r="D41">
-        <v>86.1328125</v>
+        <v>184.5703125</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>6.3829001572460813</v>
+        <v>7.7222233450308027</v>
       </c>
       <c r="B42">
-        <v>20.3946224416006</v>
+        <v>31.488905961585228</v>
       </c>
       <c r="C42">
-        <v>39.891949610176852</v>
+        <v>39.996084994565827</v>
       </c>
       <c r="D42">
-        <v>143.5546875</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>7.2135390638864729</v>
+        <v>18.43958696364691</v>
       </c>
       <c r="B43">
-        <v>21.590457733649401</v>
+        <v>53.634536188248312</v>
       </c>
       <c r="C43">
-        <v>36.456509333234692</v>
+        <v>51.999174694914409</v>
       </c>
       <c r="D43">
-        <v>103.359375</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>9.6260210979700478</v>
+        <v>7.6468955992826864</v>
       </c>
       <c r="B44">
-        <v>25.07505080532497</v>
+        <v>22.34456281936933</v>
       </c>
       <c r="C44">
-        <v>36.955946186222953</v>
+        <v>34.462563191647519</v>
       </c>
       <c r="D44">
-        <v>143.5546875</v>
+        <v>123.046875</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1148,50 +1155,50 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>6.5871535285420837</v>
+        <v>14.3965522465554</v>
       </c>
       <c r="B45">
-        <v>22.367575456786369</v>
+        <v>45.235221089484341</v>
       </c>
       <c r="C45">
-        <v>34.020614196311158</v>
+        <v>46.50779187352628</v>
       </c>
       <c r="D45">
-        <v>161.4990234375</v>
+        <v>143.5546875</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>7.8119709273937428</v>
+        <v>5.2017130672172662</v>
       </c>
       <c r="B46">
-        <v>32.453052151808997</v>
+        <v>18.257683089128051</v>
       </c>
       <c r="C46">
-        <v>36.018890659344031</v>
+        <v>32.479267181390298</v>
       </c>
       <c r="D46">
-        <v>151.9990808823529</v>
+        <v>129.19921875</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>7.7902616791126329</v>
+        <v>5.8026525179051234</v>
       </c>
       <c r="B47">
-        <v>31.63863717845387</v>
+        <v>25.75464201939657</v>
       </c>
       <c r="C47">
-        <v>37.522729055934661</v>
+        <v>36.948889560210567</v>
       </c>
       <c r="D47">
-        <v>161.4990234375</v>
+        <v>143.5546875</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1199,33 +1206,33 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>6.8372574076607124</v>
+        <v>3.2647644568862959</v>
       </c>
       <c r="B48">
-        <v>19.785642996173522</v>
+        <v>14.226692754578099</v>
       </c>
       <c r="C48">
-        <v>38.4927067156828</v>
+        <v>41.496910460179009</v>
       </c>
       <c r="D48">
-        <v>117.45383522727271</v>
+        <v>107.666015625</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>10.081317954890871</v>
+        <v>10.435630621990329</v>
       </c>
       <c r="B49">
-        <v>36.248379942108649</v>
+        <v>29.24294621450829</v>
       </c>
       <c r="C49">
-        <v>37.493748489034957</v>
+        <v>38.449738620713248</v>
       </c>
       <c r="D49">
-        <v>107.666015625</v>
+        <v>143.5546875</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1233,67 +1240,67 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>5.7096350903209281</v>
+        <v>9.8372824835755033</v>
       </c>
       <c r="B50">
-        <v>19.26767504450839</v>
+        <v>20.617251667576291</v>
       </c>
       <c r="C50">
-        <v>35.405922451983479</v>
+        <v>23.97511301585428</v>
       </c>
       <c r="D50">
-        <v>117.45383522727271</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>7.4755375520383964</v>
+        <v>5.4577732187050634</v>
       </c>
       <c r="B51">
-        <v>32.32857805140069</v>
+        <v>22.685205460569481</v>
       </c>
       <c r="C51">
-        <v>38.557239528665093</v>
+        <v>34.968029209973068</v>
       </c>
       <c r="D51">
-        <v>151.9990808823529</v>
+        <v>143.5546875</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>6.4160617029725016</v>
+        <v>5.5971591114201367</v>
       </c>
       <c r="B52">
-        <v>25.776290304986318</v>
+        <v>23.225463767527319</v>
       </c>
       <c r="C52">
-        <v>33.03652541144546</v>
+        <v>34.932298305169688</v>
       </c>
       <c r="D52">
-        <v>129.19921875</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>6.8558043357713316</v>
+        <v>6.4741871134093438</v>
       </c>
       <c r="B53">
-        <v>23.811582427088929</v>
+        <v>21.577448733102251</v>
       </c>
       <c r="C53">
-        <v>33.012258963470622</v>
+        <v>38.526859392719459</v>
       </c>
       <c r="D53">
-        <v>117.45383522727271</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1301,16 +1308,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>7.2551291434193734</v>
+        <v>6.5871535285420837</v>
       </c>
       <c r="B54">
-        <v>18.922181876889919</v>
+        <v>22.367575456786369</v>
       </c>
       <c r="C54">
-        <v>34.421107621114928</v>
+        <v>34.020614196311158</v>
       </c>
       <c r="D54">
-        <v>151.9990808823529</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1318,16 +1325,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>5.1646844904520428</v>
+        <v>5.492538208569048</v>
       </c>
       <c r="B55">
-        <v>22.183742242665168</v>
+        <v>21.556054986619959</v>
       </c>
       <c r="C55">
-        <v>37.980278169450372</v>
+        <v>34.958524604244381</v>
       </c>
       <c r="D55">
-        <v>143.5546875</v>
+        <v>86.1328125</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1335,84 +1342,84 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>4.4892834148099734</v>
+        <v>9.2706406141015378</v>
       </c>
       <c r="B56">
-        <v>19.500418732885741</v>
+        <v>28.126529384535271</v>
       </c>
       <c r="C56">
-        <v>33.897814076603701</v>
+        <v>40.976291963168961</v>
       </c>
       <c r="D56">
-        <v>172.265625</v>
+        <v>184.5703125</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>6.6377612629534131</v>
+        <v>5.2403610553127846</v>
       </c>
       <c r="B57">
-        <v>29.947387450005738</v>
+        <v>17.996925769162409</v>
       </c>
       <c r="C57">
-        <v>41.440755719398297</v>
+        <v>29.949423406457239</v>
       </c>
       <c r="D57">
-        <v>143.5546875</v>
+        <v>123.046875</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>14.99978134577416</v>
+        <v>6.0742220394265516</v>
       </c>
       <c r="B58">
-        <v>39.580362963422033</v>
+        <v>23.495997452731189</v>
       </c>
       <c r="C58">
-        <v>46.321716271358582</v>
+        <v>34.392340109396358</v>
       </c>
       <c r="D58">
-        <v>103.359375</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>4.437692449492137</v>
+        <v>3.2112575834309181</v>
       </c>
       <c r="B59">
-        <v>21.169679362928289</v>
+        <v>12.58568583176802</v>
       </c>
       <c r="C59">
-        <v>44.425417890807473</v>
+        <v>38.435627934232393</v>
       </c>
       <c r="D59">
-        <v>135.99917763157899</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>3.900149934525547</v>
+        <v>3.9127053337838391</v>
       </c>
       <c r="B60">
-        <v>7.3232414870607743</v>
+        <v>18.498457910828279</v>
       </c>
       <c r="C60">
-        <v>38.003076412401882</v>
+        <v>38.030010219648616</v>
       </c>
       <c r="D60">
-        <v>89.102909482758619</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -1420,33 +1427,33 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>7.277391978475455</v>
+        <v>6.4730211748331614</v>
       </c>
       <c r="B61">
-        <v>28.210127703077681</v>
+        <v>27.48818425779173</v>
       </c>
       <c r="C61">
-        <v>43.127577980244517</v>
+        <v>34.486773025201913</v>
       </c>
       <c r="D61">
-        <v>161.4990234375</v>
+        <v>143.5546875</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>3.09924912193032</v>
+        <v>3.99762130063435</v>
       </c>
       <c r="B62">
-        <v>15.00188022922867</v>
+        <v>19.226826771681161</v>
       </c>
       <c r="C62">
-        <v>42.917503854856363</v>
+        <v>38.95866244677935</v>
       </c>
       <c r="D62">
-        <v>143.5546875</v>
+        <v>184.5703125</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -1454,16 +1461,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>2.945462729168419</v>
+        <v>4.3347943268990914</v>
       </c>
       <c r="B63">
-        <v>12.482321293274239</v>
+        <v>21.449887292690519</v>
       </c>
       <c r="C63">
-        <v>38.476925523001547</v>
+        <v>41.921301275975082</v>
       </c>
       <c r="D63">
-        <v>172.265625</v>
+        <v>64.599609375</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -1471,33 +1478,33 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>7.4310463718355031</v>
+        <v>3.7427248416158179</v>
       </c>
       <c r="B64">
-        <v>26.517551243786979</v>
+        <v>12.107963297650761</v>
       </c>
       <c r="C64">
-        <v>37.914076430220021</v>
+        <v>33.964322679850817</v>
       </c>
       <c r="D64">
-        <v>161.4990234375</v>
+        <v>143.5546875</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>2.810516925935536</v>
+        <v>5.6269070920028046</v>
       </c>
       <c r="B65">
-        <v>12.044101190269711</v>
+        <v>24.29698571631182</v>
       </c>
       <c r="C65">
-        <v>35.930706477947169</v>
+        <v>36.001521314561607</v>
       </c>
       <c r="D65">
-        <v>258.3984375</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -1505,16 +1512,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>3.0943844017751312</v>
+        <v>3.900149934525547</v>
       </c>
       <c r="B66">
-        <v>11.88476384848779</v>
+        <v>7.3232414870607743</v>
       </c>
       <c r="C66">
-        <v>34.980884889967783</v>
+        <v>38.003076412401882</v>
       </c>
       <c r="D66">
-        <v>143.5546875</v>
+        <v>89.102909482758619</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -1522,50 +1529,50 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>2.6623723722403949</v>
+        <v>7.2551291434193734</v>
       </c>
       <c r="B67">
-        <v>9.8140449805531986</v>
+        <v>18.922181876889919</v>
       </c>
       <c r="C67">
-        <v>37.002665569007007</v>
+        <v>34.421107621114928</v>
       </c>
       <c r="D67">
-        <v>234.9076704545455</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>6.2017836082195634</v>
+        <v>10.47633707116122</v>
       </c>
       <c r="B68">
-        <v>22.15068157550828</v>
+        <v>27.097502847925739</v>
       </c>
       <c r="C68">
-        <v>33.868750721791507</v>
+        <v>39.370375152842463</v>
       </c>
       <c r="D68">
-        <v>184.5703125</v>
+        <v>129.19921875</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>6.0742220394265516</v>
+        <v>8.2107547206690707</v>
       </c>
       <c r="B69">
-        <v>23.495997452731189</v>
+        <v>24.12822156405382</v>
       </c>
       <c r="C69">
-        <v>34.392340109396358</v>
+        <v>40.987858632834808</v>
       </c>
       <c r="D69">
-        <v>135.99917763157899</v>
+        <v>123.046875</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -1573,33 +1580,33 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>2.8261850667523301</v>
+        <v>11.87667611929561</v>
       </c>
       <c r="B70">
-        <v>10.696504768214</v>
+        <v>28.87969313765354</v>
       </c>
       <c r="C70">
-        <v>41.443556269900348</v>
+        <v>44.011277749323092</v>
       </c>
       <c r="D70">
-        <v>172.265625</v>
+        <v>86.1328125</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>5.4459033401805286</v>
+        <v>3.9546209872936098</v>
       </c>
       <c r="B71">
-        <v>23.878936235811828</v>
+        <v>13.024333261232499</v>
       </c>
       <c r="C71">
-        <v>37.556639550467636</v>
+        <v>29.934003231878268</v>
       </c>
       <c r="D71">
-        <v>198.76802884615381</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -1607,84 +1614,84 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>4.9295712264293519</v>
+        <v>6.2626992706517379</v>
       </c>
       <c r="B72">
-        <v>18.86216492886436</v>
+        <v>21.081622695127869</v>
       </c>
       <c r="C72">
-        <v>31.94648746873025</v>
+        <v>35.447868406241497</v>
       </c>
       <c r="D72">
-        <v>92.28515625</v>
+        <v>123.046875</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>4.1823278754505431</v>
+        <v>6.8558043357713316</v>
       </c>
       <c r="B73">
-        <v>13.25928516135648</v>
+        <v>23.811582427088929</v>
       </c>
       <c r="C73">
-        <v>29.42007298948641</v>
+        <v>33.012258963470622</v>
       </c>
       <c r="D73">
-        <v>184.5703125</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>4.1959738527244248</v>
+        <v>12.207933978758341</v>
       </c>
       <c r="B74">
-        <v>18.589621165518309</v>
+        <v>31.158824221723918</v>
       </c>
       <c r="C74">
-        <v>33.517513802980638</v>
+        <v>43.486968097800784</v>
       </c>
       <c r="D74">
-        <v>135.99917763157899</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>3.487893461521459</v>
+        <v>10.081317954890871</v>
       </c>
       <c r="B75">
-        <v>17.322701819057549</v>
+        <v>36.248379942108649</v>
       </c>
       <c r="C75">
-        <v>31.391737829844519</v>
+        <v>37.493748489034957</v>
       </c>
       <c r="D75">
-        <v>143.5546875</v>
+        <v>107.666015625</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>5.2403610553127846</v>
+        <v>3.4114119729145251</v>
       </c>
       <c r="B76">
-        <v>17.996925769162409</v>
+        <v>13.489751573637079</v>
       </c>
       <c r="C76">
-        <v>29.949423406457239</v>
+        <v>39.447300475304459</v>
       </c>
       <c r="D76">
-        <v>123.046875</v>
+        <v>103.359375</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -1692,16 +1699,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>5.2017130672172662</v>
+        <v>4.1823278754505431</v>
       </c>
       <c r="B77">
-        <v>18.257683089128051</v>
+        <v>13.25928516135648</v>
       </c>
       <c r="C77">
-        <v>32.479267181390298</v>
+        <v>29.42007298948641</v>
       </c>
       <c r="D77">
-        <v>129.19921875</v>
+        <v>184.5703125</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -1709,33 +1716,33 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>2.9182143834007062</v>
+        <v>16.7137039099755</v>
       </c>
       <c r="B78">
-        <v>13.657347208183021</v>
+        <v>36.852265219518692</v>
       </c>
       <c r="C78">
-        <v>42.074039071318538</v>
+        <v>50.915033584508578</v>
       </c>
       <c r="D78">
-        <v>161.4990234375</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>3.6594950285650598</v>
+        <v>3.0943844017751312</v>
       </c>
       <c r="B79">
-        <v>20.019347028898181</v>
+        <v>11.88476384848779</v>
       </c>
       <c r="C79">
-        <v>35.963371476734658</v>
+        <v>34.980884889967783</v>
       </c>
       <c r="D79">
-        <v>92.28515625</v>
+        <v>143.5546875</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -1743,16 +1750,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>3.2949495057101559</v>
+        <v>27.709373913091909</v>
       </c>
       <c r="B80">
-        <v>16.15565490474296</v>
+        <v>65.752106619572231</v>
       </c>
       <c r="C80">
-        <v>36.494148416749681</v>
+        <v>56.423163316461881</v>
       </c>
       <c r="D80">
-        <v>184.5703125</v>
+        <v>123.046875</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -1760,16 +1767,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>3.2647644568862959</v>
+        <v>3.09924912193032</v>
       </c>
       <c r="B81">
-        <v>14.226692754578099</v>
+        <v>15.00188022922867</v>
       </c>
       <c r="C81">
-        <v>41.496910460179009</v>
+        <v>42.917503854856363</v>
       </c>
       <c r="D81">
-        <v>107.666015625</v>
+        <v>143.5546875</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -1777,50 +1784,50 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>7.2437476179692064</v>
+        <v>6.7123020916941467</v>
       </c>
       <c r="B82">
-        <v>22.525799102468081</v>
+        <v>21.83760329880894</v>
       </c>
       <c r="C82">
-        <v>36.501035112347417</v>
+        <v>32.519685036464637</v>
       </c>
       <c r="D82">
-        <v>151.9990808823529</v>
+        <v>143.5546875</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>3.9546209872936098</v>
+        <v>8.0217870655815702</v>
       </c>
       <c r="B83">
-        <v>13.024333261232499</v>
+        <v>22.947280559311029</v>
       </c>
       <c r="C83">
-        <v>29.934003231878268</v>
+        <v>38.458921919387009</v>
       </c>
       <c r="D83">
         <v>151.9990808823529</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>3.94072818815813</v>
+        <v>7.5198120824071637</v>
       </c>
       <c r="B84">
-        <v>16.336346397177721</v>
+        <v>21.23877946737802</v>
       </c>
       <c r="C84">
-        <v>35.468156552300393</v>
+        <v>23.023096355926249</v>
       </c>
       <c r="D84">
-        <v>151.9990808823529</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -1828,16 +1835,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>5.5971591114201367</v>
+        <v>7.2988340137923746</v>
       </c>
       <c r="B85">
-        <v>23.225463767527319</v>
+        <v>17.984033903783661</v>
       </c>
       <c r="C85">
-        <v>34.932298305169688</v>
+        <v>23.013595584347769</v>
       </c>
       <c r="D85">
-        <v>151.9990808823529</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -1845,16 +1852,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>5.6269070920028046</v>
+        <v>4.9094138830371206</v>
       </c>
       <c r="B86">
-        <v>24.29698571631182</v>
+        <v>19.699721500821521</v>
       </c>
       <c r="C86">
-        <v>36.001521314561607</v>
+        <v>34.016324322690608</v>
       </c>
       <c r="D86">
-        <v>135.99917763157899</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -1862,13 +1869,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>2.8723497250299781</v>
+        <v>3.6594950285650598</v>
       </c>
       <c r="B87">
-        <v>10.064378306225279</v>
+        <v>20.019347028898181</v>
       </c>
       <c r="C87">
-        <v>33.007807974195487</v>
+        <v>35.963371476734658</v>
       </c>
       <c r="D87">
         <v>92.28515625</v>
@@ -1879,33 +1886,33 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>3.2534303923096499</v>
+        <v>9.0272165811578589</v>
       </c>
       <c r="B88">
-        <v>12.49755402064268</v>
+        <v>27.381006255621902</v>
       </c>
       <c r="C88">
-        <v>36.968810758977483</v>
+        <v>42.523310884066412</v>
       </c>
       <c r="D88">
-        <v>184.5703125</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>3.9127053337838391</v>
+        <v>21.412058690460949</v>
       </c>
       <c r="B89">
-        <v>18.498457910828279</v>
+        <v>57.82901398006387</v>
       </c>
       <c r="C89">
-        <v>38.030010219648616</v>
+        <v>67.057395400158072</v>
       </c>
       <c r="D89">
-        <v>112.34714673913039</v>
+        <v>129.19921875</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -1913,33 +1920,33 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>3.7959054849558069</v>
+        <v>4.3243824623552696</v>
       </c>
       <c r="B90">
-        <v>17.59124137070712</v>
+        <v>17.329834019276269</v>
       </c>
       <c r="C90">
-        <v>34.363961285594833</v>
+        <v>34.003807962942879</v>
       </c>
       <c r="D90">
-        <v>215.33203125</v>
+        <v>129.19921875</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>7.3838030662323506</v>
+        <v>7.277391978475455</v>
       </c>
       <c r="B91">
-        <v>27.29515599510745</v>
+        <v>28.210127703077681</v>
       </c>
       <c r="C91">
-        <v>39.038943397243251</v>
+        <v>43.127577980244517</v>
       </c>
       <c r="D91">
-        <v>117.45383522727271</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -1947,50 +1954,50 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>7.2044853010100409</v>
+        <v>7.8119709273937428</v>
       </c>
       <c r="B92">
-        <v>25.877757403021779</v>
+        <v>32.453052151808997</v>
       </c>
       <c r="C92">
-        <v>38.498970279531967</v>
+        <v>36.018890659344031</v>
       </c>
       <c r="D92">
         <v>151.9990808823529</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>5.3101332800346839</v>
+        <v>6.092986008292697</v>
       </c>
       <c r="B93">
-        <v>24.210753664919881</v>
+        <v>19.796859119338858</v>
       </c>
       <c r="C93">
-        <v>42.027331717943639</v>
+        <v>33.01676530885608</v>
       </c>
       <c r="D93">
         <v>143.5546875</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>6.5731237961759756</v>
+        <v>6.1022749135762933</v>
       </c>
       <c r="B94">
-        <v>27.480080416714451</v>
+        <v>16.755355871137521</v>
       </c>
       <c r="C94">
-        <v>42.086367523159851</v>
+        <v>22.990994866392501</v>
       </c>
       <c r="D94">
-        <v>161.4990234375</v>
+        <v>184.5703125</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -1998,84 +2005,84 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>3.2112575834309181</v>
+        <v>6.092609462980052</v>
       </c>
       <c r="B95">
-        <v>12.58568583176802</v>
+        <v>20.34202310713675</v>
       </c>
       <c r="C95">
-        <v>38.435627934232393</v>
+        <v>34.443780104971822</v>
       </c>
       <c r="D95">
-        <v>198.76802884615381</v>
+        <v>123.046875</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>9.2891808987821385</v>
+        <v>9.0956236561017008</v>
       </c>
       <c r="B96">
-        <v>29.399520091814189</v>
+        <v>30.536121939665499</v>
       </c>
       <c r="C96">
-        <v>38.477170520338447</v>
+        <v>38.563172632784642</v>
       </c>
       <c r="D96">
-        <v>123.046875</v>
+        <v>172.265625</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>3.99762130063435</v>
+        <v>6.0182590094305048</v>
       </c>
       <c r="B97">
-        <v>19.226826771681161</v>
+        <v>17.699606603344741</v>
       </c>
       <c r="C97">
-        <v>38.95866244677935</v>
+        <v>32.464518842438899</v>
       </c>
       <c r="D97">
-        <v>184.5703125</v>
+        <v>143.5546875</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>6.1602937086877478</v>
+        <v>9.6260210979700478</v>
       </c>
       <c r="B98">
-        <v>21.600135507034889</v>
+        <v>25.07505080532497</v>
       </c>
       <c r="C98">
-        <v>33.935268214335167</v>
+        <v>36.955946186222953</v>
       </c>
       <c r="D98">
-        <v>172.265625</v>
+        <v>143.5546875</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>4.6014861104923304</v>
+        <v>7.4310463718355031</v>
       </c>
       <c r="B99">
-        <v>23.0521113403763</v>
+        <v>26.517551243786979</v>
       </c>
       <c r="C99">
-        <v>37.884638595079878</v>
+        <v>37.914076430220021</v>
       </c>
       <c r="D99">
-        <v>172.265625</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2083,67 +2090,67 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>2.6772793075222152</v>
+        <v>5.6070666806481224</v>
       </c>
       <c r="B100">
-        <v>11.16689692271737</v>
+        <v>23.253547326020861</v>
       </c>
       <c r="C100">
-        <v>36.47428110608633</v>
+        <v>34.467388321699858</v>
       </c>
       <c r="D100">
-        <v>143.5546875</v>
+        <v>172.265625</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>4.9094138830371206</v>
+        <v>11.92941465193708</v>
       </c>
       <c r="B101">
-        <v>19.699721500821521</v>
+        <v>21.34228840236667</v>
       </c>
       <c r="C101">
-        <v>34.016324322690608</v>
+        <v>27.952445402614948</v>
       </c>
       <c r="D101">
-        <v>112.34714673913039</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>5.8896558793636036</v>
+        <v>5.4802969582351251</v>
       </c>
       <c r="B102">
-        <v>22.725785395108741</v>
+        <v>18.22549514458359</v>
       </c>
       <c r="C102">
-        <v>33.892039064125093</v>
+        <v>37.903137783356136</v>
       </c>
       <c r="D102">
-        <v>129.19921875</v>
+        <v>107.666015625</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>4.0697119641583148</v>
+        <v>5.3101332800346839</v>
       </c>
       <c r="B103">
-        <v>23.866476415880321</v>
+        <v>24.210753664919881</v>
       </c>
       <c r="C103">
-        <v>41.46550028367222</v>
+        <v>42.027331717943639</v>
       </c>
       <c r="D103">
-        <v>71.77734375</v>
+        <v>143.5546875</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -2151,50 +2158,50 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>3.8419548378625761</v>
+        <v>7.2135390638864729</v>
       </c>
       <c r="B104">
-        <v>19.495951632535299</v>
+        <v>21.590457733649401</v>
       </c>
       <c r="C104">
-        <v>42.936803935067928</v>
+        <v>36.456509333234692</v>
       </c>
       <c r="D104">
-        <v>95.703125</v>
+        <v>103.359375</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>3.1196797721053122</v>
+        <v>11.486211917823489</v>
       </c>
       <c r="B105">
-        <v>14.956857826516091</v>
+        <v>34.62951404590715</v>
       </c>
       <c r="C105">
-        <v>41.047400006195453</v>
+        <v>48.069561029250607</v>
       </c>
       <c r="D105">
-        <v>161.4990234375</v>
+        <v>143.5546875</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>3.2675047207450212</v>
+        <v>6.5731237961759756</v>
       </c>
       <c r="B106">
-        <v>12.875002072191251</v>
+        <v>27.480080416714451</v>
       </c>
       <c r="C106">
-        <v>38.45829434146647</v>
+        <v>42.086367523159851</v>
       </c>
       <c r="D106">
-        <v>112.34714673913039</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -2202,67 +2209,67 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>5.4577732187050634</v>
+        <v>9.2350463989826519</v>
       </c>
       <c r="B107">
-        <v>22.685205460569481</v>
+        <v>28.751575764275319</v>
       </c>
       <c r="C107">
-        <v>34.968029209973068</v>
+        <v>37.495795349310612</v>
       </c>
       <c r="D107">
-        <v>143.5546875</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>2.8295727199177949</v>
+        <v>10.308673072178751</v>
       </c>
       <c r="B108">
-        <v>12.59001526166452</v>
+        <v>28.850810959942969</v>
       </c>
       <c r="C108">
-        <v>42.980796973193307</v>
+        <v>49.885919312899837</v>
       </c>
       <c r="D108">
-        <v>117.45383522727271</v>
+        <v>103.359375</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>3.619380328585172</v>
+        <v>16.68356557880529</v>
       </c>
       <c r="B109">
-        <v>16.507962825546901</v>
+        <v>41.620958322188947</v>
       </c>
       <c r="C109">
-        <v>38.592060599761943</v>
+        <v>48.985580429468172</v>
       </c>
       <c r="D109">
-        <v>135.99917763157899</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>3.5564046798449018</v>
+        <v>6.2017836082195634</v>
       </c>
       <c r="B110">
-        <v>15.94847817942926</v>
+        <v>22.15068157550828</v>
       </c>
       <c r="C110">
-        <v>39.915097560588983</v>
+        <v>33.868750721791507</v>
       </c>
       <c r="D110">
-        <v>161.4990234375</v>
+        <v>184.5703125</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -2270,33 +2277,33 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>8.2107547206690707</v>
+        <v>8.3301729425647597</v>
       </c>
       <c r="B111">
-        <v>24.12822156405382</v>
+        <v>32.137712447610951</v>
       </c>
       <c r="C111">
-        <v>40.987858632834808</v>
+        <v>50.001756461295628</v>
       </c>
       <c r="D111">
-        <v>123.046875</v>
+        <v>143.5546875</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>4.3347943268990914</v>
+        <v>11.28985472001454</v>
       </c>
       <c r="B112">
-        <v>21.449887292690519</v>
+        <v>57.577889392898221</v>
       </c>
       <c r="C112">
-        <v>41.921301275975082</v>
+        <v>79.428552300596081</v>
       </c>
       <c r="D112">
-        <v>64.599609375</v>
+        <v>198.76802884615381</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -2304,33 +2311,33 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>3.2955979097872778</v>
+        <v>9.3863607851169633</v>
       </c>
       <c r="B113">
-        <v>15.354512639825471</v>
+        <v>30.05943567999979</v>
       </c>
       <c r="C113">
-        <v>41.412450990211987</v>
+        <v>42.485767903670506</v>
       </c>
       <c r="D113">
-        <v>184.5703125</v>
+        <v>143.5546875</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>7.7222233450308027</v>
+        <v>5.8896558793636036</v>
       </c>
       <c r="B114">
-        <v>31.488905961585228</v>
+        <v>22.725785395108741</v>
       </c>
       <c r="C114">
-        <v>39.996084994565827</v>
+        <v>33.892039064125093</v>
       </c>
       <c r="D114">
-        <v>151.9990808823529</v>
+        <v>129.19921875</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -2338,16 +2345,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>3.0907686968562782</v>
+        <v>4.1959738527244248</v>
       </c>
       <c r="B115">
-        <v>14.82635870255192</v>
+        <v>18.589621165518309</v>
       </c>
       <c r="C115">
-        <v>40.9764986705461</v>
+        <v>33.517513802980638</v>
       </c>
       <c r="D115">
-        <v>172.265625</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -2355,13 +2362,13 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>4.3243824623552696</v>
+        <v>11.43501010074778</v>
       </c>
       <c r="B116">
-        <v>17.329834019276269</v>
+        <v>20.097487750556802</v>
       </c>
       <c r="C116">
-        <v>34.003807962942879</v>
+        <v>31.983511474034621</v>
       </c>
       <c r="D116">
         <v>129.19921875</v>
@@ -2372,16 +2379,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>15.496612233279439</v>
+        <v>8.2618677271640983</v>
       </c>
       <c r="B117">
-        <v>28.717579212558601</v>
+        <v>24.67375867885082</v>
       </c>
       <c r="C117">
-        <v>38.563911143791962</v>
+        <v>38.515744386381591</v>
       </c>
       <c r="D117">
-        <v>107.666015625</v>
+        <v>123.046875</v>
       </c>
       <c r="E117">
         <v>0</v>
@@ -2389,50 +2396,50 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>9.2782395059153391</v>
+        <v>12.224263835217609</v>
       </c>
       <c r="B118">
-        <v>31.829373132907349</v>
+        <v>25.71383238698342</v>
       </c>
       <c r="C118">
-        <v>44.548041992063332</v>
+        <v>32.970551666702782</v>
       </c>
       <c r="D118">
-        <v>123.046875</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>17.643585613099479</v>
+        <v>4.0697119641583148</v>
       </c>
       <c r="B119">
-        <v>47.196543721446879</v>
+        <v>23.866476415880321</v>
       </c>
       <c r="C119">
-        <v>58.593006567006611</v>
+        <v>41.46550028367222</v>
       </c>
       <c r="D119">
-        <v>129.19921875</v>
+        <v>71.77734375</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>5.4802969582351251</v>
+        <v>6.3829001572460813</v>
       </c>
       <c r="B120">
-        <v>18.22549514458359</v>
+        <v>20.3946224416006</v>
       </c>
       <c r="C120">
-        <v>37.903137783356136</v>
+        <v>39.891949610176852</v>
       </c>
       <c r="D120">
-        <v>107.666015625</v>
+        <v>143.5546875</v>
       </c>
       <c r="E120">
         <v>0</v>
@@ -2440,33 +2447,33 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>11.87667611929561</v>
+        <v>7.2437476179692064</v>
       </c>
       <c r="B121">
-        <v>28.87969313765354</v>
+        <v>22.525799102468081</v>
       </c>
       <c r="C121">
-        <v>44.011277749323092</v>
+        <v>36.501035112347417</v>
       </c>
       <c r="D121">
-        <v>86.1328125</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>24.30955290803595</v>
+        <v>14.99978134577416</v>
       </c>
       <c r="B122">
-        <v>51.229449548884041</v>
+        <v>39.580362963422033</v>
       </c>
       <c r="C122">
-        <v>74.583457444190088</v>
+        <v>46.321716271358582</v>
       </c>
       <c r="D122">
-        <v>117.45383522727271</v>
+        <v>103.359375</v>
       </c>
       <c r="E122">
         <v>0</v>
@@ -2474,13 +2481,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>18.608445942296299</v>
+        <v>17.643585613099479</v>
       </c>
       <c r="B123">
-        <v>39.453034853176931</v>
+        <v>47.196543721446879</v>
       </c>
       <c r="C123">
-        <v>39.499360121115828</v>
+        <v>58.593006567006611</v>
       </c>
       <c r="D123">
         <v>129.19921875</v>
@@ -2491,101 +2498,101 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>11.43501010074778</v>
+        <v>2.9182143834007062</v>
       </c>
       <c r="B124">
-        <v>20.097487750556802</v>
+        <v>13.657347208183021</v>
       </c>
       <c r="C124">
-        <v>31.983511474034621</v>
+        <v>42.074039071318538</v>
       </c>
       <c r="D124">
-        <v>129.19921875</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>9.0956236561017008</v>
+        <v>3.487893461521459</v>
       </c>
       <c r="B125">
-        <v>30.536121939665499</v>
+        <v>17.322701819057549</v>
       </c>
       <c r="C125">
-        <v>38.563172632784642</v>
+        <v>31.391737829844519</v>
       </c>
       <c r="D125">
-        <v>172.265625</v>
+        <v>143.5546875</v>
       </c>
       <c r="E125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>6.2626992706517379</v>
+        <v>3.2675047207450212</v>
       </c>
       <c r="B126">
-        <v>21.081622695127869</v>
+        <v>12.875002072191251</v>
       </c>
       <c r="C126">
-        <v>35.447868406241497</v>
+        <v>38.45829434146647</v>
       </c>
       <c r="D126">
-        <v>123.046875</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>11.57915143547722</v>
+        <v>3.619380328585172</v>
       </c>
       <c r="B127">
-        <v>19.818365200808671</v>
+        <v>16.507962825546901</v>
       </c>
       <c r="C127">
-        <v>28.533322907590762</v>
+        <v>38.592060599761943</v>
       </c>
       <c r="D127">
-        <v>129.19921875</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>8.2871666985000214</v>
+        <v>6.5381672796546173</v>
       </c>
       <c r="B128">
-        <v>21.25169668774997</v>
+        <v>16.69327069603257</v>
       </c>
       <c r="C128">
-        <v>29.116207042437029</v>
+        <v>23.983222805788991</v>
       </c>
       <c r="D128">
-        <v>112.34714673913039</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>12.141897784218539</v>
+        <v>9.4420227619200858</v>
       </c>
       <c r="B129">
-        <v>27.601770668666632</v>
+        <v>19.486697921961969</v>
       </c>
       <c r="C129">
-        <v>28.53322250024107</v>
+        <v>34.505199289614268</v>
       </c>
       <c r="D129">
-        <v>123.046875</v>
+        <v>143.5546875</v>
       </c>
       <c r="E129">
         <v>0</v>
@@ -2593,33 +2600,33 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>7.0566664626353948</v>
+        <v>25.59963862647432</v>
       </c>
       <c r="B130">
-        <v>20.50148910291761</v>
+        <v>74.467206134096088</v>
       </c>
       <c r="C130">
-        <v>24.016621854182439</v>
+        <v>71.002974822139194</v>
       </c>
       <c r="D130">
         <v>135.99917763157899</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>6.6089268378391104</v>
+        <v>6.6377612629534131</v>
       </c>
       <c r="B131">
-        <v>21.881208476677621</v>
+        <v>29.947387450005738</v>
       </c>
       <c r="C131">
-        <v>25.47330956688867</v>
+        <v>41.440755719398297</v>
       </c>
       <c r="D131">
-        <v>151.9990808823529</v>
+        <v>143.5546875</v>
       </c>
       <c r="E131">
         <v>0</v>
@@ -2627,16 +2634,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>13.08082458471026</v>
+        <v>7.9887799913592792</v>
       </c>
       <c r="B132">
-        <v>20.458707810205549</v>
+        <v>22.287395115157938</v>
       </c>
       <c r="C132">
-        <v>27.055665953878311</v>
+        <v>32.938789923250873</v>
       </c>
       <c r="D132">
-        <v>135.99917763157899</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E132">
         <v>0</v>
@@ -2644,16 +2651,16 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>11.92941465193708</v>
+        <v>5.3197985941934061</v>
       </c>
       <c r="B133">
-        <v>21.34228840236667</v>
+        <v>16.544426321543678</v>
       </c>
       <c r="C133">
-        <v>27.952445402614948</v>
+        <v>28.40577999519401</v>
       </c>
       <c r="D133">
-        <v>151.9990808823529</v>
+        <v>143.5546875</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -2661,16 +2668,16 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>4.8927031714092291</v>
+        <v>3.5564046798449018</v>
       </c>
       <c r="B134">
-        <v>23.81332129044219</v>
+        <v>15.94847817942926</v>
       </c>
       <c r="C134">
-        <v>42.509004627392891</v>
+        <v>39.915097560588983</v>
       </c>
       <c r="D134">
-        <v>123.046875</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -2678,16 +2685,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>3.4114119729145251</v>
+        <v>9.2891808987821385</v>
       </c>
       <c r="B135">
-        <v>13.489751573637079</v>
+        <v>29.399520091814189</v>
       </c>
       <c r="C135">
-        <v>39.447300475304459</v>
+        <v>38.477170520338447</v>
       </c>
       <c r="D135">
-        <v>103.359375</v>
+        <v>123.046875</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -2695,16 +2702,16 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>6.5624261916615838</v>
+        <v>3.2534303923096499</v>
       </c>
       <c r="B136">
-        <v>27.363720693581911</v>
+        <v>12.49755402064268</v>
       </c>
       <c r="C136">
-        <v>42.989934330996</v>
+        <v>36.968810758977483</v>
       </c>
       <c r="D136">
-        <v>135.99917763157899</v>
+        <v>184.5703125</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -2712,16 +2719,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>21.412058690460949</v>
+        <v>6.5624261916615838</v>
       </c>
       <c r="B137">
-        <v>57.82901398006387</v>
+        <v>27.363720693581911</v>
       </c>
       <c r="C137">
-        <v>67.057395400158072</v>
+        <v>42.989934330996</v>
       </c>
       <c r="D137">
-        <v>129.19921875</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -2729,50 +2736,50 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>25.59963862647432</v>
+        <v>7.4755375520383964</v>
       </c>
       <c r="B138">
-        <v>74.467206134096088</v>
+        <v>32.32857805140069</v>
       </c>
       <c r="C138">
-        <v>71.002974822139194</v>
+        <v>38.557239528665093</v>
       </c>
       <c r="D138">
-        <v>135.99917763157899</v>
+        <v>151.9990808823529</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>11.28985472001454</v>
+        <v>15.496612233279439</v>
       </c>
       <c r="B139">
-        <v>57.577889392898221</v>
+        <v>28.717579212558601</v>
       </c>
       <c r="C139">
-        <v>79.428552300596081</v>
+        <v>38.563911143791962</v>
       </c>
       <c r="D139">
-        <v>198.76802884615381</v>
+        <v>107.666015625</v>
       </c>
       <c r="E139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>18.43958696364691</v>
+        <v>2.8261850667523301</v>
       </c>
       <c r="B140">
-        <v>53.634536188248312</v>
+        <v>10.696504768214</v>
       </c>
       <c r="C140">
-        <v>51.999174694914409</v>
+        <v>41.443556269900348</v>
       </c>
       <c r="D140">
-        <v>151.9990808823529</v>
+        <v>172.265625</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -2780,16 +2787,16 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>14.3965522465554</v>
+        <v>3.1196797721053122</v>
       </c>
       <c r="B141">
-        <v>45.235221089484341</v>
+        <v>14.956857826516091</v>
       </c>
       <c r="C141">
-        <v>46.50779187352628</v>
+        <v>41.047400006195453</v>
       </c>
       <c r="D141">
-        <v>143.5546875</v>
+        <v>161.4990234375</v>
       </c>
       <c r="E141">
         <v>1</v>
@@ -2797,33 +2804,33 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>27.709373913091909</v>
+        <v>7.0566664626353948</v>
       </c>
       <c r="B142">
-        <v>65.752106619572231</v>
+        <v>20.50148910291761</v>
       </c>
       <c r="C142">
-        <v>56.423163316461881</v>
+        <v>24.016621854182439</v>
       </c>
       <c r="D142">
-        <v>123.046875</v>
+        <v>135.99917763157899</v>
       </c>
       <c r="E142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>9.2706406141015378</v>
+        <v>2.8295727199177949</v>
       </c>
       <c r="B143">
-        <v>28.126529384535271</v>
+        <v>12.59001526166452</v>
       </c>
       <c r="C143">
-        <v>40.976291963168961</v>
+        <v>42.980796973193307</v>
       </c>
       <c r="D143">
-        <v>184.5703125</v>
+        <v>117.45383522727271</v>
       </c>
       <c r="E143">
         <v>1</v>
@@ -2831,33 +2838,33 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>16.51834679383802</v>
+        <v>12.141897784218539</v>
       </c>
       <c r="B144">
-        <v>37.376722805629598</v>
+        <v>27.601770668666632</v>
       </c>
       <c r="C144">
-        <v>45.633330635677432</v>
+        <v>28.53322250024107</v>
       </c>
       <c r="D144">
-        <v>129.19921875</v>
+        <v>123.046875</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>9.4928905094418568</v>
+        <v>10.16534746441871</v>
       </c>
       <c r="B145">
-        <v>23.05129324263833</v>
+        <v>19.672904454870011</v>
       </c>
       <c r="C145">
-        <v>33.923142957970107</v>
+        <v>22.00061525760561</v>
       </c>
       <c r="D145">
-        <v>103.359375</v>
+        <v>112.34714673913039</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -2865,30 +2872,30 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>12.224263835217609</v>
+        <v>6.4160617029725016</v>
       </c>
       <c r="B146">
-        <v>25.71383238698342</v>
+        <v>25.776290304986318</v>
       </c>
       <c r="C146">
-        <v>32.970551666702782</v>
+        <v>33.03652541144546</v>
       </c>
       <c r="D146">
-        <v>151.9990808823529</v>
+        <v>129.19921875</v>
       </c>
       <c r="E146">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>9.8372824835755033</v>
+        <v>8.5904837391892457</v>
       </c>
       <c r="B147">
-        <v>20.617251667576291</v>
+        <v>22.67185656653098</v>
       </c>
       <c r="C147">
-        <v>23.97511301585428</v>
+        <v>22.98710423966865</v>
       </c>
       <c r="D147">
         <v>161.4990234375</v>
@@ -2899,33 +2906,33 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>7.5198120824071637</v>
+        <v>5.7096350903209281</v>
       </c>
       <c r="B148">
-        <v>21.23877946737802</v>
+        <v>19.26767504450839</v>
       </c>
       <c r="C148">
-        <v>23.023096355926249</v>
+        <v>35.405922451983479</v>
       </c>
       <c r="D148">
         <v>117.45383522727271</v>
       </c>
       <c r="E148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>10.16534746441871</v>
+        <v>3.2949495057101559</v>
       </c>
       <c r="B149">
-        <v>19.672904454870011</v>
+        <v>16.15565490474296</v>
       </c>
       <c r="C149">
-        <v>22.00061525760561</v>
+        <v>36.494148416749681</v>
       </c>
       <c r="D149">
-        <v>112.34714673913039</v>
+        <v>184.5703125</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -2933,16 +2940,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>8.5904837391892457</v>
+        <v>4.9295712264293519</v>
       </c>
       <c r="B150">
-        <v>22.67185656653098</v>
+        <v>18.86216492886436</v>
       </c>
       <c r="C150">
-        <v>22.98710423966865</v>
+        <v>31.94648746873025</v>
       </c>
       <c r="D150">
-        <v>161.4990234375</v>
+        <v>92.28515625</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -2950,50 +2957,50 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>7.2988340137923746</v>
+        <v>11.080650933467711</v>
       </c>
       <c r="B151">
-        <v>17.984033903783661</v>
+        <v>29.76354408711169</v>
       </c>
       <c r="C151">
-        <v>23.013595584347769</v>
+        <v>40.963686312294342</v>
       </c>
       <c r="D151">
         <v>198.76802884615381</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>6.1022749135762933</v>
+        <v>7.9018299084357686</v>
       </c>
       <c r="B152">
-        <v>16.755355871137521</v>
+        <v>26.280142793695109</v>
       </c>
       <c r="C152">
-        <v>22.990994866392501</v>
+        <v>37.007836202058712</v>
       </c>
       <c r="D152">
-        <v>184.5703125</v>
+        <v>107.666015625</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>6.5381672796546173</v>
+        <v>3.7959054849558069</v>
       </c>
       <c r="B153">
-        <v>16.69327069603257</v>
+        <v>17.59124137070712</v>
       </c>
       <c r="C153">
-        <v>23.983222805788991</v>
+        <v>34.363961285594833</v>
       </c>
       <c r="D153">
-        <v>161.4990234375</v>
+        <v>215.33203125</v>
       </c>
       <c r="E153">
         <v>1</v>

</xml_diff>